<commit_message>
result of the social agent
</commit_message>
<xml_diff>
--- a/data/agent_scores.xlsx
+++ b/data/agent_scores.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,35 +437,40 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Social VI</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>aggressiveBehavior</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>carefulBehavior</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>randomBehavior</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>semiAggressiveBehavior</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>semiCarefulBehavior</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>valueIterationBasedBehavior_v2</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>valueIterationBasedBehavior_v2.1</t>
         </is>
@@ -476,24 +481,27 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>25</v>
+      </c>
+      <c r="C2" t="n">
         <v>-105</v>
-      </c>
-      <c r="C2" t="n">
-        <v>20</v>
       </c>
       <c r="D2" t="n">
         <v>20</v>
       </c>
       <c r="E2" t="n">
+        <v>20</v>
+      </c>
+      <c r="F2" t="n">
         <v>-103</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>11</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>-103</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -502,24 +510,27 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>25</v>
+        <v>-103</v>
       </c>
       <c r="C3" t="n">
+        <v>25</v>
+      </c>
+      <c r="D3" t="n">
         <v>19</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>-105</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>-104</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>20</v>
       </c>
-      <c r="G3" t="n">
-        <v>25</v>
-      </c>
       <c r="H3" t="n">
+        <v>25</v>
+      </c>
+      <c r="I3" t="n">
         <v>24</v>
       </c>
     </row>
@@ -528,24 +539,27 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
+        <v>19</v>
+      </c>
+      <c r="C4" t="n">
         <v>-105</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>20</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>-135</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>-103</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>18</v>
       </c>
-      <c r="G4" t="n">
-        <v>25</v>
-      </c>
       <c r="H4" t="n">
+        <v>25</v>
+      </c>
+      <c r="I4" t="n">
         <v>25</v>
       </c>
     </row>
@@ -554,24 +568,27 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C5" t="n">
+        <v>25</v>
+      </c>
+      <c r="D5" t="n">
         <v>20</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>-110</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>-105</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>10</v>
       </c>
-      <c r="G5" t="n">
-        <v>25</v>
-      </c>
       <c r="H5" t="n">
+        <v>25</v>
+      </c>
+      <c r="I5" t="n">
         <v>-103</v>
       </c>
     </row>
@@ -580,24 +597,27 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
+        <v>22</v>
+      </c>
+      <c r="C6" t="n">
         <v>-105</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>20</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>-104</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>24</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>19</v>
       </c>
-      <c r="G6" t="n">
-        <v>25</v>
-      </c>
       <c r="H6" t="n">
+        <v>25</v>
+      </c>
+      <c r="I6" t="n">
         <v>25</v>
       </c>
     </row>
@@ -606,24 +626,27 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
+        <v>19</v>
+      </c>
+      <c r="C7" t="n">
         <v>-107</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>20</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>-111</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>-105</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>17</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>-107</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>-104</v>
       </c>
     </row>
@@ -635,21 +658,24 @@
         <v>25</v>
       </c>
       <c r="C8" t="n">
+        <v>25</v>
+      </c>
+      <c r="D8" t="n">
         <v>21</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>18</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>24</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>22</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>-108</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>25</v>
       </c>
     </row>
@@ -658,24 +684,27 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
+        <v>25</v>
+      </c>
+      <c r="C9" t="n">
         <v>-104</v>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>22</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>-116</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>-104</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>14</v>
       </c>
-      <c r="G9" t="n">
-        <v>25</v>
-      </c>
       <c r="H9" t="n">
+        <v>25</v>
+      </c>
+      <c r="I9" t="n">
         <v>25</v>
       </c>
     </row>
@@ -684,24 +713,27 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C10" t="n">
+        <v>25</v>
+      </c>
+      <c r="D10" t="n">
         <v>20</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>-105</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>-103</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>-133</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>-103</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>-104</v>
       </c>
     </row>
@@ -713,21 +745,24 @@
         <v>25</v>
       </c>
       <c r="C11" t="n">
+        <v>25</v>
+      </c>
+      <c r="D11" t="n">
         <v>20</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>22</v>
-      </c>
-      <c r="E11" t="n">
-        <v>-104</v>
       </c>
       <c r="F11" t="n">
         <v>-104</v>
       </c>
       <c r="G11" t="n">
-        <v>25</v>
+        <v>-104</v>
       </c>
       <c r="H11" t="n">
+        <v>25</v>
+      </c>
+      <c r="I11" t="n">
         <v>25</v>
       </c>
     </row>
@@ -739,21 +774,24 @@
         <v>25</v>
       </c>
       <c r="C12" t="n">
+        <v>25</v>
+      </c>
+      <c r="D12" t="n">
         <v>12</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>-109</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>-105</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>18</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>16</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>25</v>
       </c>
     </row>
@@ -762,24 +800,27 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
+        <v>-103</v>
+      </c>
+      <c r="C13" t="n">
         <v>-104</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>20</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>-110</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>24</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>6</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>23</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>25</v>
       </c>
     </row>
@@ -788,24 +829,27 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>25</v>
+        <v>-103</v>
       </c>
       <c r="C14" t="n">
+        <v>25</v>
+      </c>
+      <c r="D14" t="n">
         <v>20</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>-105</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>-104</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>18</v>
       </c>
-      <c r="G14" t="n">
-        <v>25</v>
-      </c>
       <c r="H14" t="n">
+        <v>25</v>
+      </c>
+      <c r="I14" t="n">
         <v>25</v>
       </c>
     </row>
@@ -814,24 +858,27 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
+        <v>19</v>
+      </c>
+      <c r="C15" t="n">
         <v>-103</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>20</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>-103</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>-108</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>15</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>10</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>25</v>
       </c>
     </row>
@@ -840,24 +887,27 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>25</v>
+        <v>-103</v>
       </c>
       <c r="C16" t="n">
+        <v>25</v>
+      </c>
+      <c r="D16" t="n">
         <v>22</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>-110</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>24</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>22</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>24</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>-125</v>
       </c>
     </row>
@@ -866,24 +916,27 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C17" t="n">
+        <v>25</v>
+      </c>
+      <c r="D17" t="n">
         <v>18</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>16</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>24</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>19</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>24</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>25</v>
       </c>
     </row>
@@ -895,21 +948,24 @@
         <v>25</v>
       </c>
       <c r="C18" t="n">
+        <v>25</v>
+      </c>
+      <c r="D18" t="n">
         <v>15</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>-108</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>-105</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>18</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>20</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>-103</v>
       </c>
     </row>
@@ -918,24 +974,27 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" t="n">
         <v>-103</v>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>19</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>14</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>-114</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>15</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>20</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>25</v>
       </c>
     </row>
@@ -947,22 +1006,25 @@
         <v>25</v>
       </c>
       <c r="C20" t="n">
+        <v>25</v>
+      </c>
+      <c r="D20" t="n">
         <v>20</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>21</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>-105</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>15</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>-109</v>
       </c>
-      <c r="H20" t="n">
-        <v>-104</v>
+      <c r="I20" t="n">
+        <v>-134</v>
       </c>
     </row>
     <row r="21">
@@ -970,25 +1032,28 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
+        <v>-103</v>
+      </c>
+      <c r="C21" t="n">
         <v>-104</v>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>20</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>19</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>-105</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>21</v>
       </c>
-      <c r="G21" t="n">
-        <v>25</v>
-      </c>
       <c r="H21" t="n">
         <v>25</v>
+      </c>
+      <c r="I21" t="n">
+        <v>-104</v>
       </c>
     </row>
     <row r="22">
@@ -996,25 +1061,28 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
+        <v>25</v>
+      </c>
+      <c r="C22" t="n">
         <v>-103</v>
       </c>
-      <c r="C22" t="n">
+      <c r="D22" t="n">
         <v>20</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>-106</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>24</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>22</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>21</v>
       </c>
-      <c r="H22" t="n">
-        <v>-103</v>
+      <c r="I22" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="23">
@@ -1025,21 +1093,24 @@
         <v>25</v>
       </c>
       <c r="C23" t="n">
+        <v>25</v>
+      </c>
+      <c r="D23" t="n">
         <v>20</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>-113</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>24</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>19</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>17</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>-103</v>
       </c>
     </row>
@@ -1051,21 +1122,24 @@
         <v>25</v>
       </c>
       <c r="C24" t="n">
+        <v>25</v>
+      </c>
+      <c r="D24" t="n">
         <v>22</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>-105</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>-104</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>17</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>23</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1074,25 +1148,28 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
+        <v>14</v>
+      </c>
+      <c r="C25" t="n">
         <v>-103</v>
       </c>
-      <c r="C25" t="n">
+      <c r="D25" t="n">
         <v>20</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>-104</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>24</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>13</v>
       </c>
-      <c r="G25" t="n">
-        <v>25</v>
-      </c>
       <c r="H25" t="n">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="I25" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="26">
@@ -1103,21 +1180,24 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
+        <v>25</v>
+      </c>
+      <c r="D26" t="n">
         <v>19</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>18</v>
-      </c>
-      <c r="E26" t="n">
-        <v>-105</v>
       </c>
       <c r="F26" t="n">
         <v>-105</v>
       </c>
       <c r="G26" t="n">
-        <v>25</v>
+        <v>-105</v>
       </c>
       <c r="H26" t="n">
+        <v>25</v>
+      </c>
+      <c r="I26" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1129,21 +1209,24 @@
         <v>-103</v>
       </c>
       <c r="C27" t="n">
+        <v>-103</v>
+      </c>
+      <c r="D27" t="n">
         <v>22</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>-105</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>-104</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>17</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>10</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1152,24 +1235,27 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C28" t="n">
+        <v>25</v>
+      </c>
+      <c r="D28" t="n">
         <v>20</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>-106</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>-113</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>15</v>
       </c>
-      <c r="G28" t="n">
-        <v>25</v>
-      </c>
       <c r="H28" t="n">
+        <v>25</v>
+      </c>
+      <c r="I28" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1181,21 +1267,24 @@
         <v>25</v>
       </c>
       <c r="C29" t="n">
+        <v>25</v>
+      </c>
+      <c r="D29" t="n">
         <v>18</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>-122</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>24</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>20</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>24</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1206,20 +1295,23 @@
       <c r="B30" t="n">
         <v>25</v>
       </c>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="n">
+      <c r="C30" t="n">
+        <v>25</v>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="n">
         <v>-105</v>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>-104</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>13</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>20</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1230,20 +1322,23 @@
       <c r="B31" t="n">
         <v>25</v>
       </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="n">
+      <c r="C31" t="n">
+        <v>25</v>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="n">
         <v>-105</v>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>-104</v>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>20</v>
       </c>
-      <c r="G31" t="n">
-        <v>25</v>
-      </c>
       <c r="H31" t="n">
+        <v>25</v>
+      </c>
+      <c r="I31" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1252,23 +1347,26 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
+        <v>-103</v>
+      </c>
+      <c r="C32" t="n">
         <v>-105</v>
       </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="n">
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="n">
         <v>-107</v>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>24</v>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>19</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>14</v>
       </c>
-      <c r="H32" t="n">
-        <v>25</v>
+      <c r="I32" t="n">
+        <v>-103</v>
       </c>
     </row>
     <row r="33">
@@ -1276,23 +1374,26 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C33" t="n">
         <v>-103</v>
       </c>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="n">
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="n">
         <v>-107</v>
       </c>
-      <c r="E33" t="n">
+      <c r="F33" t="n">
         <v>-104</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>20</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>-103</v>
       </c>
-      <c r="H33" t="n">
-        <v>25</v>
+      <c r="I33" t="n">
+        <v>-112</v>
       </c>
     </row>
     <row r="34">
@@ -1300,23 +1401,26 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>25</v>
-      </c>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="n">
+        <v>11</v>
+      </c>
+      <c r="C34" t="n">
+        <v>25</v>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="n">
         <v>-152</v>
       </c>
-      <c r="E34" t="n">
+      <c r="F34" t="n">
         <v>-104</v>
-      </c>
-      <c r="F34" t="n">
-        <v>17</v>
       </c>
       <c r="G34" t="n">
         <v>17</v>
       </c>
       <c r="H34" t="n">
-        <v>-103</v>
+        <v>17</v>
+      </c>
+      <c r="I34" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="35">
@@ -1326,20 +1430,23 @@
       <c r="B35" t="n">
         <v>25</v>
       </c>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="n">
+      <c r="C35" t="n">
+        <v>25</v>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="n">
         <v>21</v>
       </c>
-      <c r="E35" t="n">
+      <c r="F35" t="n">
         <v>-104</v>
       </c>
-      <c r="F35" t="n">
+      <c r="G35" t="n">
         <v>22</v>
       </c>
-      <c r="G35" t="n">
+      <c r="H35" t="n">
         <v>23</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1350,18 +1457,21 @@
       <c r="B36" t="n">
         <v>25</v>
       </c>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="n">
+      <c r="C36" t="n">
+        <v>25</v>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="n">
         <v>19</v>
       </c>
-      <c r="E36" t="n">
+      <c r="F36" t="n">
         <v>-105</v>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>13</v>
       </c>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="n">
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1370,20 +1480,23 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>25</v>
-      </c>
-      <c r="C37" t="inlineStr"/>
-      <c r="D37" t="n">
+        <v>15</v>
+      </c>
+      <c r="C37" t="n">
+        <v>25</v>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="n">
         <v>13</v>
       </c>
-      <c r="E37" t="n">
+      <c r="F37" t="n">
         <v>-103</v>
       </c>
-      <c r="F37" t="n">
+      <c r="G37" t="n">
         <v>22</v>
       </c>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="n">
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1392,21 +1505,24 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
+        <v>25</v>
+      </c>
+      <c r="C38" t="n">
         <v>-103</v>
       </c>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="n">
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="n">
         <v>21</v>
       </c>
-      <c r="E38" t="n">
+      <c r="F38" t="n">
         <v>-104</v>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>19</v>
       </c>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="n">
-        <v>-112</v>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="39">
@@ -1416,19 +1532,22 @@
       <c r="B39" t="n">
         <v>25</v>
       </c>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="n">
+      <c r="C39" t="n">
+        <v>25</v>
+      </c>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="n">
         <v>-146</v>
       </c>
-      <c r="E39" t="n">
+      <c r="F39" t="n">
         <v>24</v>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>17</v>
       </c>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="n">
-        <v>25</v>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="n">
+        <v>-103</v>
       </c>
     </row>
     <row r="40">
@@ -1438,19 +1557,22 @@
       <c r="B40" t="n">
         <v>25</v>
       </c>
-      <c r="C40" t="inlineStr"/>
-      <c r="D40" t="n">
+      <c r="C40" t="n">
+        <v>25</v>
+      </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="n">
         <v>-111</v>
       </c>
-      <c r="E40" t="n">
+      <c r="F40" t="n">
         <v>-104</v>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>21</v>
       </c>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="n">
-        <v>10</v>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="41">
@@ -1460,18 +1582,21 @@
       <c r="B41" t="n">
         <v>25</v>
       </c>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="n">
+      <c r="C41" t="n">
+        <v>25</v>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="n">
         <v>-109</v>
       </c>
-      <c r="E41" t="n">
+      <c r="F41" t="n">
         <v>24</v>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>19</v>
       </c>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="n">
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1480,21 +1605,24 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
+        <v>-107</v>
+      </c>
+      <c r="C42" t="n">
         <v>-103</v>
       </c>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="n">
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="n">
         <v>13</v>
       </c>
-      <c r="E42" t="n">
+      <c r="F42" t="n">
         <v>24</v>
       </c>
-      <c r="F42" t="n">
+      <c r="G42" t="n">
         <v>11</v>
       </c>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="n">
-        <v>25</v>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="43">
@@ -1504,19 +1632,22 @@
       <c r="B43" t="n">
         <v>25</v>
       </c>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="n">
+      <c r="C43" t="n">
+        <v>25</v>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="n">
         <v>21</v>
       </c>
-      <c r="E43" t="n">
+      <c r="F43" t="n">
         <v>24</v>
       </c>
-      <c r="F43" t="n">
+      <c r="G43" t="n">
         <v>14</v>
       </c>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="n">
-        <v>25</v>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="44">
@@ -1524,20 +1655,23 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>25</v>
-      </c>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="n">
+        <v>-103</v>
+      </c>
+      <c r="C44" t="n">
+        <v>25</v>
+      </c>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="n">
         <v>-107</v>
       </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
         <v>-105</v>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>8</v>
       </c>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="n">
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1548,19 +1682,22 @@
       <c r="B45" t="n">
         <v>25</v>
       </c>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="n">
+      <c r="C45" t="n">
+        <v>25</v>
+      </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="n">
         <v>-107</v>
       </c>
-      <c r="E45" t="n">
+      <c r="F45" t="n">
         <v>-103</v>
       </c>
-      <c r="F45" t="n">
+      <c r="G45" t="n">
         <v>21</v>
       </c>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="n">
-        <v>24</v>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="n">
+        <v>-108</v>
       </c>
     </row>
     <row r="46">
@@ -1570,18 +1707,21 @@
       <c r="B46" t="n">
         <v>25</v>
       </c>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="n">
+      <c r="C46" t="n">
+        <v>25</v>
+      </c>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="n">
         <v>-111</v>
       </c>
-      <c r="E46" t="n">
+      <c r="F46" t="n">
         <v>-104</v>
       </c>
-      <c r="F46" t="n">
+      <c r="G46" t="n">
         <v>19</v>
       </c>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="n">
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1592,19 +1732,22 @@
       <c r="B47" t="n">
         <v>25</v>
       </c>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="n">
+      <c r="C47" t="n">
+        <v>25</v>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="n">
         <v>-112</v>
       </c>
-      <c r="E47" t="n">
+      <c r="F47" t="n">
         <v>-105</v>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>13</v>
       </c>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="n">
-        <v>25</v>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="n">
+        <v>-103</v>
       </c>
     </row>
     <row r="48">
@@ -1612,21 +1755,24 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
+        <v>25</v>
+      </c>
+      <c r="C48" t="n">
         <v>-108</v>
       </c>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="n">
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="n">
         <v>-107</v>
       </c>
-      <c r="E48" t="n">
+      <c r="F48" t="n">
         <v>24</v>
       </c>
-      <c r="F48" t="n">
+      <c r="G48" t="n">
         <v>18</v>
       </c>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="n">
-        <v>25</v>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="n">
+        <v>-104</v>
       </c>
     </row>
     <row r="49">
@@ -1634,21 +1780,24 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>25</v>
-      </c>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="n">
+        <v>19</v>
+      </c>
+      <c r="C49" t="n">
+        <v>25</v>
+      </c>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="n">
         <v>-111</v>
       </c>
-      <c r="E49" t="n">
+      <c r="F49" t="n">
         <v>-103</v>
       </c>
-      <c r="F49" t="n">
+      <c r="G49" t="n">
         <v>17</v>
       </c>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="n">
-        <v>25</v>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="n">
+        <v>24</v>
       </c>
     </row>
     <row r="50">
@@ -1658,19 +1807,22 @@
       <c r="B50" t="n">
         <v>25</v>
       </c>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="n">
+      <c r="C50" t="n">
+        <v>25</v>
+      </c>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="n">
         <v>-119</v>
       </c>
-      <c r="E50" t="n">
+      <c r="F50" t="n">
         <v>-104</v>
       </c>
-      <c r="F50" t="n">
+      <c r="G50" t="n">
         <v>17</v>
       </c>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="n">
-        <v>23</v>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="51">
@@ -1680,19 +1832,22 @@
       <c r="B51" t="n">
         <v>25</v>
       </c>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="n">
+      <c r="C51" t="n">
+        <v>25</v>
+      </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="n">
         <v>-109</v>
       </c>
-      <c r="E51" t="n">
+      <c r="F51" t="n">
         <v>-104</v>
       </c>
-      <c r="F51" t="n">
+      <c r="G51" t="n">
         <v>15</v>
       </c>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="n">
-        <v>25</v>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="n">
+        <v>-103</v>
       </c>
     </row>
     <row r="52">
@@ -1702,19 +1857,22 @@
       <c r="B52" t="n">
         <v>25</v>
       </c>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="n">
+      <c r="C52" t="n">
+        <v>25</v>
+      </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="n">
         <v>-107</v>
       </c>
-      <c r="E52" t="n">
-        <v>25</v>
-      </c>
       <c r="F52" t="n">
+        <v>25</v>
+      </c>
+      <c r="G52" t="n">
         <v>16</v>
       </c>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="n">
-        <v>12</v>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="n">
+        <v>25</v>
       </c>
     </row>
     <row r="53">
@@ -1722,22 +1880,23 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
+        <v>25</v>
+      </c>
+      <c r="C53" t="n">
         <v>-103</v>
       </c>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="n">
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="n">
         <v>-107</v>
       </c>
-      <c r="E53" t="n">
+      <c r="F53" t="n">
         <v>-105</v>
       </c>
-      <c r="F53" t="n">
+      <c r="G53" t="n">
         <v>17</v>
       </c>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="n">
-        <v>25</v>
-      </c>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1746,86 +1905,90 @@
       <c r="B54" t="n">
         <v>25</v>
       </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="n">
+      <c r="C54" t="n">
+        <v>25</v>
+      </c>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="n">
         <v>-107</v>
       </c>
-      <c r="E54" t="n">
+      <c r="F54" t="n">
         <v>-109</v>
       </c>
-      <c r="F54" t="n">
+      <c r="G54" t="n">
         <v>2</v>
       </c>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="n">
-        <v>25</v>
-      </c>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>25</v>
-      </c>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="n">
+        <v>12</v>
+      </c>
+      <c r="C55" t="n">
+        <v>25</v>
+      </c>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="n">
         <v>-107</v>
       </c>
-      <c r="E55" t="n">
+      <c r="F55" t="n">
         <v>24</v>
       </c>
-      <c r="F55" t="n">
+      <c r="G55" t="n">
         <v>20</v>
       </c>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="n">
-        <v>-108</v>
-      </c>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>25</v>
-      </c>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="n">
+        <v>24</v>
+      </c>
+      <c r="C56" t="n">
+        <v>25</v>
+      </c>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="n">
         <v>-107</v>
       </c>
-      <c r="E56" t="n">
+      <c r="F56" t="n">
         <v>-104</v>
       </c>
-      <c r="F56" t="n">
+      <c r="G56" t="n">
         <v>-124</v>
       </c>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="n">
-        <v>25</v>
-      </c>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>25</v>
-      </c>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="n">
+        <v>-110</v>
+      </c>
+      <c r="C57" t="n">
+        <v>25</v>
+      </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="n">
         <v>-107</v>
       </c>
-      <c r="E57" t="n">
+      <c r="F57" t="n">
         <v>-104</v>
       </c>
-      <c r="F57" t="n">
+      <c r="G57" t="n">
         <v>-113</v>
       </c>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="n">
-        <v>-103</v>
-      </c>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1834,20 +1997,21 @@
       <c r="B58" t="n">
         <v>25</v>
       </c>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="n">
+      <c r="C58" t="n">
+        <v>25</v>
+      </c>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="n">
         <v>-107</v>
       </c>
-      <c r="E58" t="n">
+      <c r="F58" t="n">
         <v>24</v>
       </c>
-      <c r="F58" t="n">
+      <c r="G58" t="n">
         <v>-113</v>
       </c>
-      <c r="G58" t="inlineStr"/>
-      <c r="H58" t="n">
-        <v>-104</v>
-      </c>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -1856,20 +2020,21 @@
       <c r="B59" t="n">
         <v>25</v>
       </c>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="n">
+      <c r="C59" t="n">
+        <v>25</v>
+      </c>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="n">
         <v>-110</v>
       </c>
-      <c r="E59" t="n">
+      <c r="F59" t="n">
         <v>24</v>
       </c>
-      <c r="F59" t="n">
+      <c r="G59" t="n">
         <v>22</v>
       </c>
-      <c r="G59" t="inlineStr"/>
-      <c r="H59" t="n">
-        <v>25</v>
-      </c>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -1878,42 +2043,42 @@
       <c r="B60" t="n">
         <v>25</v>
       </c>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="n">
+      <c r="C60" t="n">
+        <v>25</v>
+      </c>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="n">
         <v>16</v>
       </c>
-      <c r="E60" t="n">
+      <c r="F60" t="n">
         <v>24</v>
       </c>
-      <c r="F60" t="n">
+      <c r="G60" t="n">
         <v>20</v>
       </c>
-      <c r="G60" t="inlineStr"/>
-      <c r="H60" t="n">
-        <v>25</v>
-      </c>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
       <c r="B61" t="n">
+        <v>20</v>
+      </c>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="n">
         <v>-107</v>
       </c>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="n">
-        <v>-107</v>
-      </c>
-      <c r="E61" t="n">
+      <c r="F61" t="n">
         <v>-105</v>
       </c>
-      <c r="F61" t="n">
+      <c r="G61" t="n">
         <v>14</v>
       </c>
-      <c r="G61" t="inlineStr"/>
-      <c r="H61" t="n">
-        <v>-103</v>
-      </c>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -1921,19 +2086,18 @@
       </c>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr"/>
-      <c r="D62" t="n">
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="n">
         <v>-110</v>
       </c>
-      <c r="E62" t="n">
+      <c r="F62" t="n">
         <v>-103</v>
       </c>
-      <c r="F62" t="n">
+      <c r="G62" t="n">
         <v>20</v>
       </c>
-      <c r="G62" t="inlineStr"/>
-      <c r="H62" t="n">
-        <v>25</v>
-      </c>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -1941,17 +2105,18 @@
       </c>
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr"/>
-      <c r="D63" t="n">
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="n">
         <v>21</v>
       </c>
-      <c r="E63" t="n">
+      <c r="F63" t="n">
         <v>-109</v>
       </c>
-      <c r="F63" t="n">
+      <c r="G63" t="n">
         <v>21</v>
       </c>
-      <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -1959,17 +2124,18 @@
       </c>
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr"/>
-      <c r="D64" t="n">
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="n">
         <v>-107</v>
       </c>
-      <c r="E64" t="n">
+      <c r="F64" t="n">
         <v>24</v>
       </c>
-      <c r="F64" t="n">
+      <c r="G64" t="n">
         <v>15</v>
       </c>
-      <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -1977,17 +2143,18 @@
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
-      <c r="D65" t="n">
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="n">
         <v>-107</v>
       </c>
-      <c r="E65" t="n">
+      <c r="F65" t="n">
         <v>24</v>
       </c>
-      <c r="F65" t="n">
+      <c r="G65" t="n">
         <v>-107</v>
       </c>
-      <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -1995,17 +2162,18 @@
       </c>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
-      <c r="D66" t="n">
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="n">
         <v>-107</v>
       </c>
-      <c r="E66" t="n">
+      <c r="F66" t="n">
         <v>-105</v>
       </c>
-      <c r="F66" t="n">
+      <c r="G66" t="n">
         <v>20</v>
       </c>
-      <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2013,17 +2181,18 @@
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
-      <c r="D67" t="n">
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="n">
         <v>5</v>
       </c>
-      <c r="E67" t="n">
+      <c r="F67" t="n">
         <v>-105</v>
       </c>
-      <c r="F67" t="n">
+      <c r="G67" t="n">
         <v>-137</v>
       </c>
-      <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2032,14 +2201,15 @@
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr"/>
-      <c r="E68" t="n">
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="n">
         <v>24</v>
       </c>
-      <c r="F68" t="n">
+      <c r="G68" t="n">
         <v>17</v>
       </c>
-      <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2048,14 +2218,15 @@
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
-      <c r="E69" t="n">
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="n">
         <v>24</v>
       </c>
-      <c r="F69" t="n">
+      <c r="G69" t="n">
         <v>-136</v>
       </c>
-      <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2064,14 +2235,15 @@
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr"/>
-      <c r="E70" t="n">
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="n">
         <v>-104</v>
       </c>
-      <c r="F70" t="n">
+      <c r="G70" t="n">
         <v>17</v>
       </c>
-      <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2080,14 +2252,15 @@
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr"/>
-      <c r="E71" t="n">
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="n">
         <v>24</v>
       </c>
-      <c r="F71" t="n">
+      <c r="G71" t="n">
         <v>12</v>
       </c>
-      <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2096,14 +2269,15 @@
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
-      <c r="E72" t="n">
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="n">
         <v>-107</v>
       </c>
-      <c r="F72" t="n">
+      <c r="G72" t="n">
         <v>-106</v>
       </c>
-      <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2112,14 +2286,15 @@
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr"/>
-      <c r="E73" t="n">
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="n">
         <v>24</v>
       </c>
-      <c r="F73" t="n">
+      <c r="G73" t="n">
         <v>9</v>
       </c>
-      <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2128,14 +2303,15 @@
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr"/>
-      <c r="E74" t="n">
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="n">
         <v>-105</v>
       </c>
-      <c r="F74" t="n">
+      <c r="G74" t="n">
         <v>20</v>
       </c>
-      <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2144,14 +2320,15 @@
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr"/>
-      <c r="E75" t="n">
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="n">
         <v>24</v>
       </c>
-      <c r="F75" t="n">
+      <c r="G75" t="n">
         <v>-111</v>
       </c>
-      <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2160,14 +2337,15 @@
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr"/>
-      <c r="E76" t="n">
+      <c r="E76" t="inlineStr"/>
+      <c r="F76" t="n">
         <v>-104</v>
       </c>
-      <c r="F76" t="n">
+      <c r="G76" t="n">
         <v>19</v>
       </c>
-      <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -2176,14 +2354,15 @@
       <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr"/>
-      <c r="E77" t="n">
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="n">
         <v>-107</v>
       </c>
-      <c r="F77" t="n">
+      <c r="G77" t="n">
         <v>17</v>
       </c>
-      <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2192,14 +2371,15 @@
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr"/>
-      <c r="E78" t="n">
+      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="n">
         <v>-104</v>
       </c>
-      <c r="F78" t="n">
+      <c r="G78" t="n">
         <v>17</v>
       </c>
-      <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2212,7 +2392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H78"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2223,35 +2403,40 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Social VI</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>aggressiveBehavior</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>carefulBehavior</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>randomBehavior</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>semiAggressiveBehavior</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>semiCarefulBehavior</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>valueIterationBasedBehavior_v2</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>valueIterationBasedBehavior_v2.1</t>
         </is>
@@ -2262,24 +2447,27 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>43</v>
+      </c>
+      <c r="C2" t="n">
         <v>-210</v>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>43</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>40</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>-206</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>17</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>-206</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>46</v>
       </c>
     </row>
@@ -2288,24 +2476,27 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
+        <v>-206</v>
+      </c>
+      <c r="C3" t="n">
         <v>46</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>41</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>-210</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>-208</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>43</v>
       </c>
-      <c r="G3" t="n">
-        <v>48</v>
-      </c>
       <c r="H3" t="n">
+        <v>48</v>
+      </c>
+      <c r="I3" t="n">
         <v>39</v>
       </c>
     </row>
@@ -2314,24 +2505,27 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
+        <v>39</v>
+      </c>
+      <c r="C4" t="n">
         <v>-210</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>43</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>-270</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>-206</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>39</v>
       </c>
-      <c r="G4" t="n">
-        <v>48</v>
-      </c>
       <c r="H4" t="n">
+        <v>48</v>
+      </c>
+      <c r="I4" t="n">
         <v>47</v>
       </c>
     </row>
@@ -2340,24 +2534,27 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C5" t="n">
+        <v>48</v>
+      </c>
+      <c r="D5" t="n">
         <v>43</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>-220</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>-210</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>23</v>
       </c>
-      <c r="G5" t="n">
-        <v>47</v>
-      </c>
       <c r="H5" t="n">
+        <v>47</v>
+      </c>
+      <c r="I5" t="n">
         <v>-206</v>
       </c>
     </row>
@@ -2366,24 +2563,27 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
+        <v>45</v>
+      </c>
+      <c r="C6" t="n">
         <v>-210</v>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>40</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>-208</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>43</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>41</v>
       </c>
-      <c r="G6" t="n">
-        <v>47</v>
-      </c>
       <c r="H6" t="n">
+        <v>47</v>
+      </c>
+      <c r="I6" t="n">
         <v>44</v>
       </c>
     </row>
@@ -2392,24 +2592,27 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
+        <v>26</v>
+      </c>
+      <c r="C7" t="n">
         <v>-214</v>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>43</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>-222</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>-210</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>36</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>-214</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>-208</v>
       </c>
     </row>
@@ -2418,24 +2621,27 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" t="n">
+        <v>48</v>
+      </c>
+      <c r="D8" t="n">
         <v>44</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>38</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>45</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>40</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>-216</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>48</v>
       </c>
     </row>
@@ -2444,24 +2650,27 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
+        <v>48</v>
+      </c>
+      <c r="C9" t="n">
         <v>-208</v>
       </c>
-      <c r="C9" t="n">
-        <v>47</v>
-      </c>
       <c r="D9" t="n">
+        <v>47</v>
+      </c>
+      <c r="E9" t="n">
         <v>-232</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>-208</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>31</v>
       </c>
-      <c r="G9" t="n">
-        <v>47</v>
-      </c>
       <c r="H9" t="n">
+        <v>47</v>
+      </c>
+      <c r="I9" t="n">
         <v>45</v>
       </c>
     </row>
@@ -2470,24 +2679,27 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C10" t="n">
+        <v>47</v>
+      </c>
+      <c r="D10" t="n">
         <v>43</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>-210</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>-206</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>-266</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>-206</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>-208</v>
       </c>
     </row>
@@ -2496,24 +2708,27 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" t="n">
+        <v>48</v>
+      </c>
+      <c r="D11" t="n">
         <v>43</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>45</v>
-      </c>
-      <c r="E11" t="n">
-        <v>-208</v>
       </c>
       <c r="F11" t="n">
         <v>-208</v>
       </c>
       <c r="G11" t="n">
-        <v>48</v>
+        <v>-208</v>
       </c>
       <c r="H11" t="n">
+        <v>48</v>
+      </c>
+      <c r="I11" t="n">
         <v>48</v>
       </c>
     </row>
@@ -2525,21 +2740,24 @@
         <v>48</v>
       </c>
       <c r="C12" t="n">
+        <v>48</v>
+      </c>
+      <c r="D12" t="n">
         <v>24</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>-218</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>-210</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>39</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>33</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>47</v>
       </c>
     </row>
@@ -2548,24 +2766,27 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
+        <v>-206</v>
+      </c>
+      <c r="C13" t="n">
         <v>-208</v>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>43</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>-220</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>45</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>15</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>43</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>48</v>
       </c>
     </row>
@@ -2574,24 +2795,27 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
+        <v>-206</v>
+      </c>
+      <c r="C14" t="n">
         <v>46</v>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>43</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>-210</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>-208</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>39</v>
       </c>
-      <c r="G14" t="n">
-        <v>47</v>
-      </c>
       <c r="H14" t="n">
+        <v>47</v>
+      </c>
+      <c r="I14" t="n">
         <v>48</v>
       </c>
     </row>
@@ -2600,24 +2824,27 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
+        <v>39</v>
+      </c>
+      <c r="C15" t="n">
         <v>-206</v>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>43</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>-206</v>
       </c>
-      <c r="E15" t="n">
+      <c r="F15" t="n">
         <v>-216</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>33</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>23</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>48</v>
       </c>
     </row>
@@ -2626,24 +2853,27 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>47</v>
+        <v>-206</v>
       </c>
       <c r="C16" t="n">
         <v>47</v>
       </c>
       <c r="D16" t="n">
+        <v>47</v>
+      </c>
+      <c r="E16" t="n">
         <v>-220</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>43</v>
       </c>
-      <c r="F16" t="n">
-        <v>47</v>
-      </c>
       <c r="G16" t="n">
+        <v>47</v>
+      </c>
+      <c r="H16" t="n">
         <v>49</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>-250</v>
       </c>
     </row>
@@ -2652,24 +2882,27 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C17" t="n">
+        <v>48</v>
+      </c>
+      <c r="D17" t="n">
         <v>39</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>36</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>43</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>40</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>49</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>45</v>
       </c>
     </row>
@@ -2681,21 +2914,24 @@
         <v>47</v>
       </c>
       <c r="C18" t="n">
+        <v>47</v>
+      </c>
+      <c r="D18" t="n">
         <v>33</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>-216</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>-210</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>39</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>43</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>-206</v>
       </c>
     </row>
@@ -2704,24 +2940,27 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
+        <v>-3</v>
+      </c>
+      <c r="C19" t="n">
         <v>-206</v>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>40</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>30</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>-228</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>32</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>41</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>46</v>
       </c>
     </row>
@@ -2730,25 +2969,28 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" t="n">
+        <v>47</v>
+      </c>
+      <c r="D20" t="n">
         <v>43</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>46</v>
       </c>
-      <c r="E20" t="n">
+      <c r="F20" t="n">
         <v>-210</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>33</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>-218</v>
       </c>
-      <c r="H20" t="n">
-        <v>-208</v>
+      <c r="I20" t="n">
+        <v>-268</v>
       </c>
     </row>
     <row r="21">
@@ -2756,25 +2998,28 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
+        <v>-206</v>
+      </c>
+      <c r="C21" t="n">
         <v>-208</v>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>43</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>42</v>
       </c>
-      <c r="E21" t="n">
+      <c r="F21" t="n">
         <v>-210</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>45</v>
       </c>
-      <c r="G21" t="n">
-        <v>48</v>
-      </c>
       <c r="H21" t="n">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="I21" t="n">
+        <v>-208</v>
       </c>
     </row>
     <row r="22">
@@ -2782,25 +3027,28 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
+        <v>47</v>
+      </c>
+      <c r="C22" t="n">
         <v>-206</v>
       </c>
-      <c r="C22" t="n">
+      <c r="D22" t="n">
         <v>43</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>-212</v>
       </c>
-      <c r="E22" t="n">
+      <c r="F22" t="n">
         <v>45</v>
       </c>
-      <c r="F22" t="n">
-        <v>47</v>
-      </c>
       <c r="G22" t="n">
+        <v>47</v>
+      </c>
+      <c r="H22" t="n">
         <v>40</v>
       </c>
-      <c r="H22" t="n">
-        <v>-206</v>
+      <c r="I22" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="23">
@@ -2811,21 +3059,24 @@
         <v>48</v>
       </c>
       <c r="C23" t="n">
+        <v>48</v>
+      </c>
+      <c r="D23" t="n">
         <v>43</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>-226</v>
       </c>
-      <c r="E23" t="n">
+      <c r="F23" t="n">
         <v>45</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>41</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>31</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>-206</v>
       </c>
     </row>
@@ -2834,24 +3085,27 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24" t="n">
         <v>47</v>
       </c>
       <c r="D24" t="n">
+        <v>47</v>
+      </c>
+      <c r="E24" t="n">
         <v>-210</v>
       </c>
-      <c r="E24" t="n">
+      <c r="F24" t="n">
         <v>-208</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>37</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>44</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>48</v>
       </c>
     </row>
@@ -2860,25 +3114,28 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
+        <v>29</v>
+      </c>
+      <c r="C25" t="n">
         <v>-206</v>
       </c>
-      <c r="C25" t="n">
+      <c r="D25" t="n">
         <v>43</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>-208</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>45</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>28</v>
       </c>
-      <c r="G25" t="n">
-        <v>47</v>
-      </c>
       <c r="H25" t="n">
-        <v>41</v>
+        <v>47</v>
+      </c>
+      <c r="I25" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="26">
@@ -2886,25 +3143,28 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" t="n">
+        <v>48</v>
+      </c>
+      <c r="D26" t="n">
         <v>40</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>39</v>
-      </c>
-      <c r="E26" t="n">
-        <v>-210</v>
       </c>
       <c r="F26" t="n">
         <v>-210</v>
       </c>
       <c r="G26" t="n">
-        <v>48</v>
+        <v>-210</v>
       </c>
       <c r="H26" t="n">
         <v>48</v>
+      </c>
+      <c r="I26" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="27">
@@ -2915,21 +3175,24 @@
         <v>-206</v>
       </c>
       <c r="C27" t="n">
-        <v>47</v>
+        <v>-206</v>
       </c>
       <c r="D27" t="n">
+        <v>47</v>
+      </c>
+      <c r="E27" t="n">
         <v>-210</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>-208</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>36</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>23</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>48</v>
       </c>
     </row>
@@ -2938,25 +3201,28 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C28" t="n">
+        <v>48</v>
+      </c>
+      <c r="D28" t="n">
         <v>43</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>-212</v>
       </c>
-      <c r="E28" t="n">
+      <c r="F28" t="n">
         <v>-226</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>33</v>
       </c>
-      <c r="G28" t="n">
-        <v>48</v>
-      </c>
       <c r="H28" t="n">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="I28" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="29">
@@ -2964,25 +3230,28 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
+        <v>47</v>
+      </c>
+      <c r="C29" t="n">
         <v>44</v>
       </c>
-      <c r="C29" t="n">
+      <c r="D29" t="n">
         <v>39</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>-244</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>45</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>43</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>45</v>
       </c>
-      <c r="H29" t="n">
-        <v>48</v>
+      <c r="I29" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="30">
@@ -2990,23 +3259,26 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>47</v>
-      </c>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="n">
+        <v>44</v>
+      </c>
+      <c r="C30" t="n">
+        <v>47</v>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="n">
         <v>-210</v>
       </c>
-      <c r="E30" t="n">
+      <c r="F30" t="n">
         <v>-208</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>13</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>43</v>
       </c>
-      <c r="H30" t="n">
-        <v>48</v>
+      <c r="I30" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="31">
@@ -3016,21 +3288,24 @@
       <c r="B31" t="n">
         <v>47</v>
       </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="n">
+      <c r="C31" t="n">
+        <v>47</v>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="n">
         <v>-210</v>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>-208</v>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>43</v>
       </c>
-      <c r="G31" t="n">
-        <v>48</v>
-      </c>
       <c r="H31" t="n">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="I31" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="32">
@@ -3038,23 +3313,26 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
+        <v>-206</v>
+      </c>
+      <c r="C32" t="n">
         <v>-210</v>
       </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="n">
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="n">
         <v>-214</v>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>43</v>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>40</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>28</v>
       </c>
-      <c r="H32" t="n">
-        <v>45</v>
+      <c r="I32" t="n">
+        <v>-206</v>
       </c>
     </row>
     <row r="33">
@@ -3062,23 +3340,26 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
+        <v>-3</v>
+      </c>
+      <c r="C33" t="n">
         <v>-206</v>
       </c>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="n">
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="n">
         <v>-214</v>
       </c>
-      <c r="E33" t="n">
+      <c r="F33" t="n">
         <v>-208</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>43</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>-206</v>
       </c>
-      <c r="H33" t="n">
-        <v>46</v>
+      <c r="I33" t="n">
+        <v>-224</v>
       </c>
     </row>
     <row r="34">
@@ -3086,23 +3367,26 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>47</v>
-      </c>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="n">
+        <v>23</v>
+      </c>
+      <c r="C34" t="n">
+        <v>47</v>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="n">
         <v>-304</v>
       </c>
-      <c r="E34" t="n">
+      <c r="F34" t="n">
         <v>-208</v>
-      </c>
-      <c r="F34" t="n">
-        <v>37</v>
       </c>
       <c r="G34" t="n">
         <v>37</v>
       </c>
       <c r="H34" t="n">
-        <v>-206</v>
+        <v>37</v>
+      </c>
+      <c r="I34" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="35">
@@ -3112,20 +3396,23 @@
       <c r="B35" t="n">
         <v>47</v>
       </c>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="n">
+      <c r="C35" t="n">
+        <v>47</v>
+      </c>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="n">
         <v>46</v>
       </c>
-      <c r="E35" t="n">
+      <c r="F35" t="n">
         <v>-208</v>
       </c>
-      <c r="F35" t="n">
-        <v>47</v>
-      </c>
       <c r="G35" t="n">
+        <v>47</v>
+      </c>
+      <c r="H35" t="n">
         <v>44</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>47</v>
       </c>
     </row>
@@ -3136,19 +3423,22 @@
       <c r="B36" t="n">
         <v>48</v>
       </c>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="n">
+      <c r="C36" t="n">
+        <v>48</v>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="n">
         <v>42</v>
       </c>
-      <c r="E36" t="n">
+      <c r="F36" t="n">
         <v>-210</v>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>29</v>
       </c>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="n">
-        <v>45</v>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="37">
@@ -3156,20 +3446,23 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>48</v>
-      </c>
-      <c r="C37" t="inlineStr"/>
-      <c r="D37" t="n">
+        <v>31</v>
+      </c>
+      <c r="C37" t="n">
+        <v>48</v>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="n">
         <v>30</v>
       </c>
-      <c r="E37" t="n">
+      <c r="F37" t="n">
         <v>-206</v>
       </c>
-      <c r="F37" t="n">
-        <v>47</v>
-      </c>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="n">
+      <c r="G37" t="n">
+        <v>47</v>
+      </c>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="n">
         <v>46</v>
       </c>
     </row>
@@ -3178,21 +3471,24 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
+        <v>47</v>
+      </c>
+      <c r="C38" t="n">
         <v>-206</v>
       </c>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="n">
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="n">
         <v>46</v>
       </c>
-      <c r="E38" t="n">
+      <c r="F38" t="n">
         <v>-208</v>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>41</v>
       </c>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="n">
-        <v>-224</v>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="n">
+        <v>48</v>
       </c>
     </row>
     <row r="39">
@@ -3200,21 +3496,24 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
+        <v>48</v>
+      </c>
+      <c r="C39" t="n">
         <v>36</v>
       </c>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="n">
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="n">
         <v>-292</v>
       </c>
-      <c r="E39" t="n">
+      <c r="F39" t="n">
         <v>45</v>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>37</v>
       </c>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="n">
-        <v>47</v>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="n">
+        <v>-206</v>
       </c>
     </row>
     <row r="40">
@@ -3222,21 +3521,24 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>47</v>
-      </c>
-      <c r="C40" t="inlineStr"/>
-      <c r="D40" t="n">
+        <v>46</v>
+      </c>
+      <c r="C40" t="n">
+        <v>47</v>
+      </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="n">
         <v>-222</v>
       </c>
-      <c r="E40" t="n">
+      <c r="F40" t="n">
         <v>-208</v>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>42</v>
       </c>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="n">
-        <v>15</v>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="41">
@@ -3244,20 +3546,23 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>47</v>
-      </c>
-      <c r="C41" t="inlineStr"/>
-      <c r="D41" t="n">
+        <v>48</v>
+      </c>
+      <c r="C41" t="n">
+        <v>47</v>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="n">
         <v>-218</v>
       </c>
-      <c r="E41" t="n">
+      <c r="F41" t="n">
         <v>45</v>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>41</v>
       </c>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="n">
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="n">
         <v>47</v>
       </c>
     </row>
@@ -3266,21 +3571,24 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
+        <v>-214</v>
+      </c>
+      <c r="C42" t="n">
         <v>-206</v>
       </c>
-      <c r="C42" t="inlineStr"/>
-      <c r="D42" t="n">
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="n">
         <v>30</v>
       </c>
-      <c r="E42" t="n">
+      <c r="F42" t="n">
         <v>45</v>
       </c>
-      <c r="F42" t="n">
-        <v>25</v>
-      </c>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="n">
-        <v>46</v>
+      <c r="G42" t="n">
+        <v>25</v>
+      </c>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="43">
@@ -3288,21 +3596,24 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>47</v>
-      </c>
-      <c r="C43" t="inlineStr"/>
-      <c r="D43" t="n">
+        <v>43</v>
+      </c>
+      <c r="C43" t="n">
+        <v>47</v>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="n">
         <v>46</v>
       </c>
-      <c r="E43" t="n">
+      <c r="F43" t="n">
         <v>45</v>
       </c>
-      <c r="F43" t="n">
+      <c r="G43" t="n">
         <v>30</v>
       </c>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="n">
-        <v>46</v>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="44">
@@ -3310,20 +3621,23 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>47</v>
-      </c>
-      <c r="C44" t="inlineStr"/>
-      <c r="D44" t="n">
+        <v>-206</v>
+      </c>
+      <c r="C44" t="n">
+        <v>47</v>
+      </c>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="n">
         <v>-214</v>
       </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
         <v>-210</v>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>18</v>
       </c>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="n">
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="n">
         <v>48</v>
       </c>
     </row>
@@ -3332,21 +3646,24 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
+        <v>48</v>
+      </c>
+      <c r="C45" t="n">
         <v>44</v>
       </c>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="n">
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="n">
         <v>-214</v>
       </c>
-      <c r="E45" t="n">
+      <c r="F45" t="n">
         <v>-206</v>
       </c>
-      <c r="F45" t="n">
+      <c r="G45" t="n">
         <v>43</v>
       </c>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="n">
-        <v>46</v>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="n">
+        <v>-216</v>
       </c>
     </row>
     <row r="46">
@@ -3354,21 +3671,24 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
+        <v>45</v>
+      </c>
+      <c r="C46" t="n">
         <v>46</v>
       </c>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="n">
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="n">
         <v>-222</v>
       </c>
-      <c r="E46" t="n">
+      <c r="F46" t="n">
         <v>-208</v>
       </c>
-      <c r="F46" t="n">
+      <c r="G46" t="n">
         <v>41</v>
       </c>
-      <c r="G46" t="inlineStr"/>
-      <c r="H46" t="n">
-        <v>46</v>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="n">
+        <v>47</v>
       </c>
     </row>
     <row r="47">
@@ -3378,19 +3698,22 @@
       <c r="B47" t="n">
         <v>47</v>
       </c>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="n">
+      <c r="C47" t="n">
+        <v>47</v>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="n">
         <v>-224</v>
       </c>
-      <c r="E47" t="n">
+      <c r="F47" t="n">
         <v>-210</v>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>29</v>
       </c>
-      <c r="G47" t="inlineStr"/>
-      <c r="H47" t="n">
-        <v>48</v>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="n">
+        <v>-206</v>
       </c>
     </row>
     <row r="48">
@@ -3398,21 +3721,24 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
+        <v>47</v>
+      </c>
+      <c r="C48" t="n">
         <v>-216</v>
       </c>
-      <c r="C48" t="inlineStr"/>
-      <c r="D48" t="n">
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="n">
         <v>-214</v>
       </c>
-      <c r="E48" t="n">
+      <c r="F48" t="n">
         <v>45</v>
       </c>
-      <c r="F48" t="n">
+      <c r="G48" t="n">
         <v>33</v>
       </c>
-      <c r="G48" t="inlineStr"/>
-      <c r="H48" t="n">
-        <v>47</v>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="n">
+        <v>-208</v>
       </c>
     </row>
     <row r="49">
@@ -3420,21 +3746,24 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
+        <v>39</v>
+      </c>
+      <c r="C49" t="n">
         <v>45</v>
       </c>
-      <c r="C49" t="inlineStr"/>
-      <c r="D49" t="n">
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="n">
         <v>-222</v>
       </c>
-      <c r="E49" t="n">
+      <c r="F49" t="n">
         <v>-206</v>
       </c>
-      <c r="F49" t="n">
+      <c r="G49" t="n">
         <v>36</v>
       </c>
-      <c r="G49" t="inlineStr"/>
-      <c r="H49" t="n">
-        <v>47</v>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="50">
@@ -3442,21 +3771,24 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
+        <v>48</v>
+      </c>
+      <c r="C50" t="n">
         <v>46</v>
       </c>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="n">
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="n">
         <v>-238</v>
       </c>
-      <c r="E50" t="n">
+      <c r="F50" t="n">
         <v>-208</v>
       </c>
-      <c r="F50" t="n">
+      <c r="G50" t="n">
         <v>37</v>
       </c>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="n">
-        <v>35</v>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="n">
+        <v>44</v>
       </c>
     </row>
     <row r="51">
@@ -3466,19 +3798,22 @@
       <c r="B51" t="n">
         <v>48</v>
       </c>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="n">
+      <c r="C51" t="n">
+        <v>48</v>
+      </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="n">
         <v>-218</v>
       </c>
-      <c r="E51" t="n">
+      <c r="F51" t="n">
         <v>-208</v>
       </c>
-      <c r="F51" t="n">
+      <c r="G51" t="n">
         <v>32</v>
       </c>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="n">
-        <v>48</v>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="n">
+        <v>-206</v>
       </c>
     </row>
     <row r="52">
@@ -3486,21 +3821,24 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>48</v>
-      </c>
-      <c r="C52" t="inlineStr"/>
-      <c r="D52" t="n">
+        <v>47</v>
+      </c>
+      <c r="C52" t="n">
+        <v>48</v>
+      </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="n">
         <v>-214</v>
       </c>
-      <c r="E52" t="n">
+      <c r="F52" t="n">
         <v>45</v>
       </c>
-      <c r="F52" t="n">
+      <c r="G52" t="n">
         <v>35</v>
       </c>
-      <c r="G52" t="inlineStr"/>
-      <c r="H52" t="n">
-        <v>22</v>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="n">
+        <v>46</v>
       </c>
     </row>
     <row r="53">
@@ -3508,22 +3846,23 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
+        <v>48</v>
+      </c>
+      <c r="C53" t="n">
         <v>-206</v>
       </c>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="n">
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="n">
         <v>-214</v>
       </c>
-      <c r="E53" t="n">
+      <c r="F53" t="n">
         <v>-210</v>
       </c>
-      <c r="F53" t="n">
+      <c r="G53" t="n">
         <v>37</v>
       </c>
-      <c r="G53" t="inlineStr"/>
-      <c r="H53" t="n">
-        <v>45</v>
-      </c>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -3532,86 +3871,90 @@
       <c r="B54" t="n">
         <v>47</v>
       </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="n">
+      <c r="C54" t="n">
+        <v>47</v>
+      </c>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="n">
         <v>-214</v>
       </c>
-      <c r="E54" t="n">
+      <c r="F54" t="n">
         <v>-218</v>
       </c>
-      <c r="F54" t="n">
+      <c r="G54" t="n">
         <v>4</v>
       </c>
-      <c r="G54" t="inlineStr"/>
-      <c r="H54" t="n">
-        <v>48</v>
-      </c>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>48</v>
-      </c>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="n">
+        <v>25</v>
+      </c>
+      <c r="C55" t="n">
+        <v>48</v>
+      </c>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="n">
         <v>-214</v>
       </c>
-      <c r="E55" t="n">
+      <c r="F55" t="n">
         <v>46</v>
       </c>
-      <c r="F55" t="n">
+      <c r="G55" t="n">
         <v>43</v>
       </c>
-      <c r="G55" t="inlineStr"/>
-      <c r="H55" t="n">
-        <v>-216</v>
-      </c>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>47</v>
-      </c>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="n">
+        <v>45</v>
+      </c>
+      <c r="C56" t="n">
+        <v>47</v>
+      </c>
+      <c r="D56" t="inlineStr"/>
+      <c r="E56" t="n">
         <v>-214</v>
       </c>
-      <c r="E56" t="n">
+      <c r="F56" t="n">
         <v>-208</v>
       </c>
-      <c r="F56" t="n">
+      <c r="G56" t="n">
         <v>-248</v>
       </c>
-      <c r="G56" t="inlineStr"/>
-      <c r="H56" t="n">
-        <v>47</v>
-      </c>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>47</v>
-      </c>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="n">
+        <v>-220</v>
+      </c>
+      <c r="C57" t="n">
+        <v>47</v>
+      </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="n">
         <v>-214</v>
       </c>
-      <c r="E57" t="n">
+      <c r="F57" t="n">
         <v>-208</v>
       </c>
-      <c r="F57" t="n">
+      <c r="G57" t="n">
         <v>-226</v>
       </c>
-      <c r="G57" t="inlineStr"/>
-      <c r="H57" t="n">
-        <v>-206</v>
-      </c>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -3620,86 +3963,88 @@
       <c r="B58" t="n">
         <v>48</v>
       </c>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="n">
+      <c r="C58" t="n">
+        <v>48</v>
+      </c>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="n">
         <v>-214</v>
       </c>
-      <c r="E58" t="n">
+      <c r="F58" t="n">
         <v>45</v>
       </c>
-      <c r="F58" t="n">
+      <c r="G58" t="n">
         <v>-226</v>
       </c>
-      <c r="G58" t="inlineStr"/>
-      <c r="H58" t="n">
-        <v>-208</v>
-      </c>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>48</v>
-      </c>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="n">
+        <v>47</v>
+      </c>
+      <c r="C59" t="n">
+        <v>48</v>
+      </c>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="n">
         <v>-220</v>
       </c>
-      <c r="E59" t="n">
+      <c r="F59" t="n">
         <v>46</v>
       </c>
-      <c r="F59" t="n">
-        <v>47</v>
-      </c>
-      <c r="G59" t="inlineStr"/>
-      <c r="H59" t="n">
-        <v>48</v>
-      </c>
+      <c r="G59" t="n">
+        <v>47</v>
+      </c>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>48</v>
-      </c>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="n">
+        <v>45</v>
+      </c>
+      <c r="C60" t="n">
+        <v>48</v>
+      </c>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="n">
         <v>33</v>
       </c>
-      <c r="E60" t="n">
+      <c r="F60" t="n">
         <v>45</v>
       </c>
-      <c r="F60" t="n">
+      <c r="G60" t="n">
         <v>43</v>
       </c>
-      <c r="G60" t="inlineStr"/>
-      <c r="H60" t="n">
-        <v>44</v>
-      </c>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
       <c r="B61" t="n">
+        <v>41</v>
+      </c>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="n">
         <v>-214</v>
       </c>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="n">
-        <v>-214</v>
-      </c>
-      <c r="E61" t="n">
+      <c r="F61" t="n">
         <v>-210</v>
       </c>
-      <c r="F61" t="n">
+      <c r="G61" t="n">
         <v>30</v>
       </c>
-      <c r="G61" t="inlineStr"/>
-      <c r="H61" t="n">
-        <v>-206</v>
-      </c>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
@@ -3707,19 +4052,18 @@
       </c>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr"/>
-      <c r="D62" t="n">
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="n">
         <v>-220</v>
       </c>
-      <c r="E62" t="n">
+      <c r="F62" t="n">
         <v>-206</v>
       </c>
-      <c r="F62" t="n">
+      <c r="G62" t="n">
         <v>43</v>
       </c>
-      <c r="G62" t="inlineStr"/>
-      <c r="H62" t="n">
-        <v>46</v>
-      </c>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -3727,17 +4071,18 @@
       </c>
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr"/>
-      <c r="D63" t="n">
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="n">
         <v>46</v>
       </c>
-      <c r="E63" t="n">
+      <c r="F63" t="n">
         <v>-218</v>
       </c>
-      <c r="F63" t="n">
+      <c r="G63" t="n">
         <v>45</v>
       </c>
-      <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -3745,17 +4090,18 @@
       </c>
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr"/>
-      <c r="D64" t="n">
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="n">
         <v>-214</v>
       </c>
-      <c r="E64" t="n">
+      <c r="F64" t="n">
         <v>45</v>
       </c>
-      <c r="F64" t="n">
+      <c r="G64" t="n">
         <v>33</v>
       </c>
-      <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -3763,17 +4109,18 @@
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
-      <c r="D65" t="n">
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="n">
         <v>-214</v>
       </c>
-      <c r="E65" t="n">
+      <c r="F65" t="n">
         <v>45</v>
       </c>
-      <c r="F65" t="n">
+      <c r="G65" t="n">
         <v>-214</v>
       </c>
-      <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -3781,17 +4128,18 @@
       </c>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
-      <c r="D66" t="n">
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="n">
         <v>-214</v>
       </c>
-      <c r="E66" t="n">
+      <c r="F66" t="n">
         <v>-210</v>
       </c>
-      <c r="F66" t="n">
+      <c r="G66" t="n">
         <v>43</v>
       </c>
-      <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -3799,17 +4147,18 @@
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
-      <c r="D67" t="n">
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="n">
         <v>12</v>
       </c>
-      <c r="E67" t="n">
+      <c r="F67" t="n">
         <v>-210</v>
       </c>
-      <c r="F67" t="n">
+      <c r="G67" t="n">
         <v>-274</v>
       </c>
-      <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -3818,14 +4167,15 @@
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
       <c r="D68" t="inlineStr"/>
-      <c r="E68" t="n">
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="n">
         <v>43</v>
       </c>
-      <c r="F68" t="n">
+      <c r="G68" t="n">
         <v>37</v>
       </c>
-      <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -3834,14 +4184,15 @@
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
       <c r="D69" t="inlineStr"/>
-      <c r="E69" t="n">
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="n">
         <v>43</v>
       </c>
-      <c r="F69" t="n">
+      <c r="G69" t="n">
         <v>-272</v>
       </c>
-      <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -3850,14 +4201,15 @@
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
       <c r="D70" t="inlineStr"/>
-      <c r="E70" t="n">
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="n">
         <v>-208</v>
       </c>
-      <c r="F70" t="n">
+      <c r="G70" t="n">
         <v>37</v>
       </c>
-      <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -3866,14 +4218,15 @@
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
       <c r="D71" t="inlineStr"/>
-      <c r="E71" t="n">
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="n">
         <v>45</v>
       </c>
-      <c r="F71" t="n">
+      <c r="G71" t="n">
         <v>26</v>
       </c>
-      <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -3882,14 +4235,15 @@
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
-      <c r="E72" t="n">
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="n">
         <v>-214</v>
       </c>
-      <c r="F72" t="n">
+      <c r="G72" t="n">
         <v>-212</v>
       </c>
-      <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -3898,14 +4252,15 @@
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr"/>
-      <c r="E73" t="n">
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="n">
         <v>46</v>
       </c>
-      <c r="F73" t="n">
+      <c r="G73" t="n">
         <v>21</v>
       </c>
-      <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -3914,14 +4269,15 @@
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr"/>
-      <c r="E74" t="n">
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="n">
         <v>-210</v>
       </c>
-      <c r="F74" t="n">
+      <c r="G74" t="n">
         <v>42</v>
       </c>
-      <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -3930,14 +4286,15 @@
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr"/>
-      <c r="E75" t="n">
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="n">
         <v>46</v>
       </c>
-      <c r="F75" t="n">
+      <c r="G75" t="n">
         <v>-222</v>
       </c>
-      <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -3946,14 +4303,15 @@
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr"/>
-      <c r="E76" t="n">
+      <c r="E76" t="inlineStr"/>
+      <c r="F76" t="n">
         <v>-208</v>
       </c>
-      <c r="F76" t="n">
+      <c r="G76" t="n">
         <v>41</v>
       </c>
-      <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -3962,14 +4320,15 @@
       <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr"/>
-      <c r="E77" t="n">
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="n">
         <v>-214</v>
       </c>
-      <c r="F77" t="n">
+      <c r="G77" t="n">
         <v>37</v>
       </c>
-      <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -3978,14 +4337,15 @@
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr"/>
-      <c r="E78" t="n">
+      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="n">
         <v>-208</v>
       </c>
-      <c r="F78" t="n">
+      <c r="G78" t="n">
         <v>36</v>
       </c>
-      <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
add id for each batch in df
</commit_message>
<xml_diff>
--- a/data/agent_scores.xlsx
+++ b/data/agent_scores.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,40 +437,35 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Social VI</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>aggressiveBehavior</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>carefulBehavior</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>randomBehavior</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>semiAggressiveBehavior</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>semiCarefulBehavior</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>valueIterationBasedBehavior_v2</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>valueIterationBasedBehavior_v2.1</t>
         </is>
@@ -481,27 +476,24 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>25</v>
+        <v>-105</v>
       </c>
       <c r="C2" t="n">
-        <v>-105</v>
+        <v>20</v>
       </c>
       <c r="D2" t="n">
         <v>20</v>
       </c>
       <c r="E2" t="n">
-        <v>20</v>
+        <v>-103</v>
       </c>
       <c r="F2" t="n">
+        <v>11</v>
+      </c>
+      <c r="G2" t="n">
         <v>-103</v>
       </c>
-      <c r="G2" t="n">
-        <v>11</v>
-      </c>
       <c r="H2" t="n">
-        <v>-103</v>
-      </c>
-      <c r="I2" t="n">
         <v>25</v>
       </c>
     </row>
@@ -510,27 +502,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-103</v>
+        <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D3" t="n">
-        <v>19</v>
+        <v>-105</v>
       </c>
       <c r="E3" t="n">
-        <v>-105</v>
+        <v>-104</v>
       </c>
       <c r="F3" t="n">
-        <v>-104</v>
+        <v>20</v>
       </c>
       <c r="G3" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H3" t="n">
-        <v>25</v>
-      </c>
-      <c r="I3" t="n">
         <v>24</v>
       </c>
     </row>
@@ -539,27 +528,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>19</v>
+        <v>-105</v>
       </c>
       <c r="C4" t="n">
-        <v>-105</v>
+        <v>20</v>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>-135</v>
       </c>
       <c r="E4" t="n">
-        <v>-135</v>
+        <v>-103</v>
       </c>
       <c r="F4" t="n">
-        <v>-103</v>
+        <v>18</v>
       </c>
       <c r="G4" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H4" t="n">
-        <v>25</v>
-      </c>
-      <c r="I4" t="n">
         <v>25</v>
       </c>
     </row>
@@ -568,27 +554,24 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
+        <v>25</v>
+      </c>
+      <c r="C5" t="n">
+        <v>20</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-110</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-105</v>
+      </c>
+      <c r="F5" t="n">
         <v>10</v>
       </c>
-      <c r="C5" t="n">
-        <v>25</v>
-      </c>
-      <c r="D5" t="n">
-        <v>20</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-110</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-105</v>
-      </c>
       <c r="G5" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="H5" t="n">
-        <v>25</v>
-      </c>
-      <c r="I5" t="n">
         <v>-103</v>
       </c>
     </row>
@@ -597,27 +580,24 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>22</v>
+        <v>-105</v>
       </c>
       <c r="C6" t="n">
-        <v>-105</v>
+        <v>20</v>
       </c>
       <c r="D6" t="n">
-        <v>20</v>
+        <v>-104</v>
       </c>
       <c r="E6" t="n">
-        <v>-104</v>
+        <v>24</v>
       </c>
       <c r="F6" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G6" t="n">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H6" t="n">
-        <v>25</v>
-      </c>
-      <c r="I6" t="n">
         <v>25</v>
       </c>
     </row>
@@ -626,27 +606,24 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>19</v>
+        <v>-107</v>
       </c>
       <c r="C7" t="n">
+        <v>20</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-111</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-105</v>
+      </c>
+      <c r="F7" t="n">
+        <v>17</v>
+      </c>
+      <c r="G7" t="n">
         <v>-107</v>
       </c>
-      <c r="D7" t="n">
-        <v>20</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-111</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-105</v>
-      </c>
-      <c r="G7" t="n">
-        <v>17</v>
-      </c>
       <c r="H7" t="n">
-        <v>-107</v>
-      </c>
-      <c r="I7" t="n">
         <v>-104</v>
       </c>
     </row>
@@ -658,24 +635,21 @@
         <v>25</v>
       </c>
       <c r="C8" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E8" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F8" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G8" t="n">
-        <v>22</v>
+        <v>-108</v>
       </c>
       <c r="H8" t="n">
-        <v>-108</v>
-      </c>
-      <c r="I8" t="n">
         <v>25</v>
       </c>
     </row>
@@ -684,27 +658,24 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>25</v>
+        <v>-104</v>
       </c>
       <c r="C9" t="n">
+        <v>22</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-116</v>
+      </c>
+      <c r="E9" t="n">
         <v>-104</v>
       </c>
-      <c r="D9" t="n">
-        <v>22</v>
-      </c>
-      <c r="E9" t="n">
-        <v>-116</v>
-      </c>
       <c r="F9" t="n">
-        <v>-104</v>
+        <v>14</v>
       </c>
       <c r="G9" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="H9" t="n">
-        <v>25</v>
-      </c>
-      <c r="I9" t="n">
         <v>25</v>
       </c>
     </row>
@@ -713,27 +684,24 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C10" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D10" t="n">
-        <v>20</v>
+        <v>-105</v>
       </c>
       <c r="E10" t="n">
-        <v>-105</v>
+        <v>-103</v>
       </c>
       <c r="F10" t="n">
+        <v>-133</v>
+      </c>
+      <c r="G10" t="n">
         <v>-103</v>
       </c>
-      <c r="G10" t="n">
-        <v>-133</v>
-      </c>
       <c r="H10" t="n">
-        <v>-103</v>
-      </c>
-      <c r="I10" t="n">
         <v>-104</v>
       </c>
     </row>
@@ -745,24 +713,21 @@
         <v>25</v>
       </c>
       <c r="C11" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D11" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E11" t="n">
-        <v>22</v>
+        <v>-104</v>
       </c>
       <c r="F11" t="n">
         <v>-104</v>
       </c>
       <c r="G11" t="n">
-        <v>-104</v>
+        <v>25</v>
       </c>
       <c r="H11" t="n">
-        <v>25</v>
-      </c>
-      <c r="I11" t="n">
         <v>25</v>
       </c>
     </row>
@@ -774,24 +739,21 @@
         <v>25</v>
       </c>
       <c r="C12" t="n">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D12" t="n">
-        <v>12</v>
+        <v>-109</v>
       </c>
       <c r="E12" t="n">
-        <v>-109</v>
+        <v>-105</v>
       </c>
       <c r="F12" t="n">
-        <v>-105</v>
+        <v>18</v>
       </c>
       <c r="G12" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H12" t="n">
-        <v>16</v>
-      </c>
-      <c r="I12" t="n">
         <v>25</v>
       </c>
     </row>
@@ -800,27 +762,24 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-103</v>
+        <v>-104</v>
       </c>
       <c r="C13" t="n">
-        <v>-104</v>
+        <v>20</v>
       </c>
       <c r="D13" t="n">
-        <v>20</v>
+        <v>-110</v>
       </c>
       <c r="E13" t="n">
-        <v>-110</v>
+        <v>24</v>
       </c>
       <c r="F13" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="G13" t="n">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="H13" t="n">
-        <v>23</v>
-      </c>
-      <c r="I13" t="n">
         <v>25</v>
       </c>
     </row>
@@ -829,27 +788,24 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-103</v>
+        <v>25</v>
       </c>
       <c r="C14" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D14" t="n">
-        <v>20</v>
+        <v>-105</v>
       </c>
       <c r="E14" t="n">
-        <v>-105</v>
+        <v>-104</v>
       </c>
       <c r="F14" t="n">
-        <v>-104</v>
+        <v>18</v>
       </c>
       <c r="G14" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H14" t="n">
-        <v>25</v>
-      </c>
-      <c r="I14" t="n">
         <v>25</v>
       </c>
     </row>
@@ -858,27 +814,24 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>19</v>
+        <v>-103</v>
       </c>
       <c r="C15" t="n">
+        <v>20</v>
+      </c>
+      <c r="D15" t="n">
         <v>-103</v>
       </c>
-      <c r="D15" t="n">
-        <v>20</v>
-      </c>
       <c r="E15" t="n">
-        <v>-103</v>
+        <v>-108</v>
       </c>
       <c r="F15" t="n">
-        <v>-108</v>
+        <v>15</v>
       </c>
       <c r="G15" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H15" t="n">
-        <v>10</v>
-      </c>
-      <c r="I15" t="n">
         <v>25</v>
       </c>
     </row>
@@ -887,27 +840,24 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-103</v>
+        <v>25</v>
       </c>
       <c r="C16" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D16" t="n">
+        <v>-110</v>
+      </c>
+      <c r="E16" t="n">
+        <v>24</v>
+      </c>
+      <c r="F16" t="n">
         <v>22</v>
       </c>
-      <c r="E16" t="n">
-        <v>-110</v>
-      </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>24</v>
       </c>
-      <c r="G16" t="n">
-        <v>22</v>
-      </c>
       <c r="H16" t="n">
-        <v>24</v>
-      </c>
-      <c r="I16" t="n">
         <v>-125</v>
       </c>
     </row>
@@ -916,27 +866,24 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
+        <v>25</v>
+      </c>
+      <c r="C17" t="n">
         <v>18</v>
       </c>
-      <c r="C17" t="n">
-        <v>25</v>
-      </c>
       <c r="D17" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E17" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F17" t="n">
+        <v>19</v>
+      </c>
+      <c r="G17" t="n">
         <v>24</v>
       </c>
-      <c r="G17" t="n">
-        <v>19</v>
-      </c>
       <c r="H17" t="n">
-        <v>24</v>
-      </c>
-      <c r="I17" t="n">
         <v>25</v>
       </c>
     </row>
@@ -948,24 +895,21 @@
         <v>25</v>
       </c>
       <c r="C18" t="n">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D18" t="n">
-        <v>15</v>
+        <v>-108</v>
       </c>
       <c r="E18" t="n">
-        <v>-108</v>
+        <v>-105</v>
       </c>
       <c r="F18" t="n">
-        <v>-105</v>
+        <v>18</v>
       </c>
       <c r="G18" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H18" t="n">
-        <v>20</v>
-      </c>
-      <c r="I18" t="n">
         <v>-103</v>
       </c>
     </row>
@@ -974,27 +918,24 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>-103</v>
       </c>
       <c r="C19" t="n">
-        <v>-103</v>
+        <v>19</v>
       </c>
       <c r="D19" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E19" t="n">
-        <v>14</v>
+        <v>-114</v>
       </c>
       <c r="F19" t="n">
-        <v>-114</v>
+        <v>15</v>
       </c>
       <c r="G19" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H19" t="n">
-        <v>20</v>
-      </c>
-      <c r="I19" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1006,24 +947,21 @@
         <v>25</v>
       </c>
       <c r="C20" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D20" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E20" t="n">
-        <v>21</v>
+        <v>-105</v>
       </c>
       <c r="F20" t="n">
-        <v>-105</v>
+        <v>15</v>
       </c>
       <c r="G20" t="n">
-        <v>15</v>
+        <v>-109</v>
       </c>
       <c r="H20" t="n">
-        <v>-109</v>
-      </c>
-      <c r="I20" t="n">
         <v>-134</v>
       </c>
     </row>
@@ -1032,27 +970,24 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-103</v>
+        <v>-104</v>
       </c>
       <c r="C21" t="n">
-        <v>-104</v>
+        <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" t="n">
-        <v>19</v>
+        <v>-105</v>
       </c>
       <c r="F21" t="n">
-        <v>-105</v>
+        <v>21</v>
       </c>
       <c r="G21" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H21" t="n">
-        <v>25</v>
-      </c>
-      <c r="I21" t="n">
         <v>-104</v>
       </c>
     </row>
@@ -1061,27 +996,24 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>25</v>
+        <v>-103</v>
       </c>
       <c r="C22" t="n">
-        <v>-103</v>
+        <v>20</v>
       </c>
       <c r="D22" t="n">
-        <v>20</v>
+        <v>-106</v>
       </c>
       <c r="E22" t="n">
-        <v>-106</v>
+        <v>24</v>
       </c>
       <c r="F22" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G22" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H22" t="n">
-        <v>21</v>
-      </c>
-      <c r="I22" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1093,24 +1025,21 @@
         <v>25</v>
       </c>
       <c r="C23" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D23" t="n">
-        <v>20</v>
+        <v>-113</v>
       </c>
       <c r="E23" t="n">
-        <v>-113</v>
+        <v>24</v>
       </c>
       <c r="F23" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G23" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H23" t="n">
-        <v>17</v>
-      </c>
-      <c r="I23" t="n">
         <v>-103</v>
       </c>
     </row>
@@ -1122,24 +1051,21 @@
         <v>25</v>
       </c>
       <c r="C24" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D24" t="n">
-        <v>22</v>
+        <v>-105</v>
       </c>
       <c r="E24" t="n">
-        <v>-105</v>
+        <v>-104</v>
       </c>
       <c r="F24" t="n">
-        <v>-104</v>
+        <v>17</v>
       </c>
       <c r="G24" t="n">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="H24" t="n">
-        <v>23</v>
-      </c>
-      <c r="I24" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1148,27 +1074,24 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>14</v>
+        <v>-103</v>
       </c>
       <c r="C25" t="n">
-        <v>-103</v>
+        <v>20</v>
       </c>
       <c r="D25" t="n">
-        <v>20</v>
+        <v>-104</v>
       </c>
       <c r="E25" t="n">
-        <v>-104</v>
+        <v>24</v>
       </c>
       <c r="F25" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="G25" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="H25" t="n">
-        <v>25</v>
-      </c>
-      <c r="I25" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1180,24 +1103,21 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D26" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E26" t="n">
-        <v>18</v>
+        <v>-105</v>
       </c>
       <c r="F26" t="n">
         <v>-105</v>
       </c>
       <c r="G26" t="n">
-        <v>-105</v>
+        <v>25</v>
       </c>
       <c r="H26" t="n">
-        <v>25</v>
-      </c>
-      <c r="I26" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1209,24 +1129,21 @@
         <v>-103</v>
       </c>
       <c r="C27" t="n">
-        <v>-103</v>
+        <v>22</v>
       </c>
       <c r="D27" t="n">
-        <v>22</v>
+        <v>-105</v>
       </c>
       <c r="E27" t="n">
-        <v>-105</v>
+        <v>-104</v>
       </c>
       <c r="F27" t="n">
-        <v>-104</v>
+        <v>17</v>
       </c>
       <c r="G27" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H27" t="n">
-        <v>10</v>
-      </c>
-      <c r="I27" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1235,27 +1152,24 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C28" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D28" t="n">
-        <v>20</v>
+        <v>-106</v>
       </c>
       <c r="E28" t="n">
-        <v>-106</v>
+        <v>-113</v>
       </c>
       <c r="F28" t="n">
-        <v>-113</v>
+        <v>15</v>
       </c>
       <c r="G28" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="H28" t="n">
-        <v>25</v>
-      </c>
-      <c r="I28" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1267,24 +1181,21 @@
         <v>25</v>
       </c>
       <c r="C29" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D29" t="n">
-        <v>18</v>
+        <v>-122</v>
       </c>
       <c r="E29" t="n">
-        <v>-122</v>
+        <v>24</v>
       </c>
       <c r="F29" t="n">
+        <v>20</v>
+      </c>
+      <c r="G29" t="n">
         <v>24</v>
       </c>
-      <c r="G29" t="n">
-        <v>20</v>
-      </c>
       <c r="H29" t="n">
-        <v>24</v>
-      </c>
-      <c r="I29" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1296,22 +1207,21 @@
         <v>25</v>
       </c>
       <c r="C30" t="n">
-        <v>25</v>
-      </c>
-      <c r="D30" t="inlineStr"/>
+        <v>-118</v>
+      </c>
+      <c r="D30" t="n">
+        <v>-105</v>
+      </c>
       <c r="E30" t="n">
-        <v>-105</v>
+        <v>-104</v>
       </c>
       <c r="F30" t="n">
-        <v>-104</v>
+        <v>13</v>
       </c>
       <c r="G30" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H30" t="n">
-        <v>20</v>
-      </c>
-      <c r="I30" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1323,22 +1233,21 @@
         <v>25</v>
       </c>
       <c r="C31" t="n">
-        <v>25</v>
-      </c>
-      <c r="D31" t="inlineStr"/>
+        <v>-104</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-105</v>
+      </c>
       <c r="E31" t="n">
-        <v>-105</v>
+        <v>-104</v>
       </c>
       <c r="F31" t="n">
-        <v>-104</v>
+        <v>20</v>
       </c>
       <c r="G31" t="n">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H31" t="n">
-        <v>25</v>
-      </c>
-      <c r="I31" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1347,25 +1256,24 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-103</v>
+        <v>-105</v>
       </c>
       <c r="C32" t="n">
-        <v>-105</v>
-      </c>
-      <c r="D32" t="inlineStr"/>
+        <v>20</v>
+      </c>
+      <c r="D32" t="n">
+        <v>-107</v>
+      </c>
       <c r="E32" t="n">
-        <v>-107</v>
+        <v>24</v>
       </c>
       <c r="F32" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G32" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H32" t="n">
-        <v>14</v>
-      </c>
-      <c r="I32" t="n">
         <v>-103</v>
       </c>
     </row>
@@ -1374,25 +1282,24 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-2</v>
+        <v>-103</v>
       </c>
       <c r="C33" t="n">
+        <v>20</v>
+      </c>
+      <c r="D33" t="n">
+        <v>-107</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-104</v>
+      </c>
+      <c r="F33" t="n">
+        <v>20</v>
+      </c>
+      <c r="G33" t="n">
         <v>-103</v>
       </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="n">
-        <v>-107</v>
-      </c>
-      <c r="F33" t="n">
-        <v>-104</v>
-      </c>
-      <c r="G33" t="n">
-        <v>20</v>
-      </c>
       <c r="H33" t="n">
-        <v>-103</v>
-      </c>
-      <c r="I33" t="n">
         <v>-112</v>
       </c>
     </row>
@@ -1401,25 +1308,24 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C34" t="n">
-        <v>25</v>
-      </c>
-      <c r="D34" t="inlineStr"/>
+        <v>22</v>
+      </c>
+      <c r="D34" t="n">
+        <v>-152</v>
+      </c>
       <c r="E34" t="n">
-        <v>-152</v>
+        <v>-104</v>
       </c>
       <c r="F34" t="n">
-        <v>-104</v>
+        <v>17</v>
       </c>
       <c r="G34" t="n">
         <v>17</v>
       </c>
       <c r="H34" t="n">
-        <v>17</v>
-      </c>
-      <c r="I34" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1430,23 +1336,20 @@
       <c r="B35" t="n">
         <v>25</v>
       </c>
-      <c r="C35" t="n">
-        <v>25</v>
-      </c>
-      <c r="D35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="n">
+        <v>21</v>
+      </c>
       <c r="E35" t="n">
-        <v>21</v>
+        <v>-104</v>
       </c>
       <c r="F35" t="n">
-        <v>-104</v>
+        <v>22</v>
       </c>
       <c r="G35" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H35" t="n">
-        <v>23</v>
-      </c>
-      <c r="I35" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1457,21 +1360,20 @@
       <c r="B36" t="n">
         <v>25</v>
       </c>
-      <c r="C36" t="n">
-        <v>25</v>
-      </c>
-      <c r="D36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="n">
+        <v>19</v>
+      </c>
       <c r="E36" t="n">
-        <v>19</v>
+        <v>-105</v>
       </c>
       <c r="F36" t="n">
-        <v>-105</v>
+        <v>13</v>
       </c>
       <c r="G36" t="n">
-        <v>13</v>
-      </c>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="n">
+        <v>25</v>
+      </c>
+      <c r="H36" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1480,23 +1382,22 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>15</v>
-      </c>
-      <c r="C37" t="n">
-        <v>25</v>
-      </c>
-      <c r="D37" t="inlineStr"/>
+        <v>25</v>
+      </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="n">
+        <v>13</v>
+      </c>
       <c r="E37" t="n">
-        <v>13</v>
+        <v>-103</v>
       </c>
       <c r="F37" t="n">
-        <v>-103</v>
+        <v>22</v>
       </c>
       <c r="G37" t="n">
-        <v>22</v>
-      </c>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="n">
+        <v>25</v>
+      </c>
+      <c r="H37" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1505,23 +1406,22 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>25</v>
-      </c>
-      <c r="C38" t="n">
         <v>-103</v>
       </c>
-      <c r="D38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="n">
+        <v>21</v>
+      </c>
       <c r="E38" t="n">
-        <v>21</v>
+        <v>-104</v>
       </c>
       <c r="F38" t="n">
+        <v>19</v>
+      </c>
+      <c r="G38" t="n">
         <v>-104</v>
       </c>
-      <c r="G38" t="n">
-        <v>19</v>
-      </c>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="n">
+      <c r="H38" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1532,21 +1432,20 @@
       <c r="B39" t="n">
         <v>25</v>
       </c>
-      <c r="C39" t="n">
-        <v>25</v>
-      </c>
-      <c r="D39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="n">
+        <v>-146</v>
+      </c>
       <c r="E39" t="n">
-        <v>-146</v>
+        <v>24</v>
       </c>
       <c r="F39" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="G39" t="n">
-        <v>17</v>
-      </c>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="n">
+        <v>-145</v>
+      </c>
+      <c r="H39" t="n">
         <v>-103</v>
       </c>
     </row>
@@ -1557,21 +1456,18 @@
       <c r="B40" t="n">
         <v>25</v>
       </c>
-      <c r="C40" t="n">
-        <v>25</v>
-      </c>
-      <c r="D40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="n">
+        <v>-111</v>
+      </c>
       <c r="E40" t="n">
-        <v>-111</v>
+        <v>-104</v>
       </c>
       <c r="F40" t="n">
-        <v>-104</v>
-      </c>
-      <c r="G40" t="n">
         <v>21</v>
       </c>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="n">
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1582,21 +1478,18 @@
       <c r="B41" t="n">
         <v>25</v>
       </c>
-      <c r="C41" t="n">
-        <v>25</v>
-      </c>
-      <c r="D41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="n">
+        <v>-109</v>
+      </c>
       <c r="E41" t="n">
-        <v>-109</v>
+        <v>24</v>
       </c>
       <c r="F41" t="n">
-        <v>24</v>
-      </c>
-      <c r="G41" t="n">
         <v>19</v>
       </c>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="n">
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1605,23 +1498,20 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-107</v>
-      </c>
-      <c r="C42" t="n">
         <v>-103</v>
       </c>
-      <c r="D42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="n">
+        <v>13</v>
+      </c>
       <c r="E42" t="n">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F42" t="n">
-        <v>24</v>
-      </c>
-      <c r="G42" t="n">
         <v>11</v>
       </c>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="n">
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="n">
         <v>12</v>
       </c>
     </row>
@@ -1632,21 +1522,18 @@
       <c r="B43" t="n">
         <v>25</v>
       </c>
-      <c r="C43" t="n">
-        <v>25</v>
-      </c>
-      <c r="D43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="n">
+        <v>21</v>
+      </c>
       <c r="E43" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F43" t="n">
-        <v>24</v>
-      </c>
-      <c r="G43" t="n">
         <v>14</v>
       </c>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="n">
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1655,23 +1542,20 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>-103</v>
-      </c>
-      <c r="C44" t="n">
-        <v>25</v>
-      </c>
-      <c r="D44" t="inlineStr"/>
+        <v>25</v>
+      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="n">
+        <v>-107</v>
+      </c>
       <c r="E44" t="n">
-        <v>-107</v>
+        <v>-105</v>
       </c>
       <c r="F44" t="n">
-        <v>-105</v>
-      </c>
-      <c r="G44" t="n">
         <v>8</v>
       </c>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="n">
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1682,21 +1566,18 @@
       <c r="B45" t="n">
         <v>25</v>
       </c>
-      <c r="C45" t="n">
-        <v>25</v>
-      </c>
-      <c r="D45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="n">
+        <v>-107</v>
+      </c>
       <c r="E45" t="n">
-        <v>-107</v>
+        <v>-103</v>
       </c>
       <c r="F45" t="n">
-        <v>-103</v>
-      </c>
-      <c r="G45" t="n">
         <v>21</v>
       </c>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="n">
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="n">
         <v>-108</v>
       </c>
     </row>
@@ -1707,21 +1588,18 @@
       <c r="B46" t="n">
         <v>25</v>
       </c>
-      <c r="C46" t="n">
-        <v>25</v>
-      </c>
-      <c r="D46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="n">
+        <v>-111</v>
+      </c>
       <c r="E46" t="n">
-        <v>-111</v>
+        <v>-104</v>
       </c>
       <c r="F46" t="n">
-        <v>-104</v>
-      </c>
-      <c r="G46" t="n">
         <v>19</v>
       </c>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="n">
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1732,21 +1610,18 @@
       <c r="B47" t="n">
         <v>25</v>
       </c>
-      <c r="C47" t="n">
-        <v>25</v>
-      </c>
-      <c r="D47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="n">
+        <v>-112</v>
+      </c>
       <c r="E47" t="n">
-        <v>-112</v>
+        <v>-105</v>
       </c>
       <c r="F47" t="n">
-        <v>-105</v>
-      </c>
-      <c r="G47" t="n">
         <v>13</v>
       </c>
-      <c r="H47" t="inlineStr"/>
-      <c r="I47" t="n">
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="n">
         <v>-103</v>
       </c>
     </row>
@@ -1755,23 +1630,20 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>25</v>
-      </c>
-      <c r="C48" t="n">
         <v>-108</v>
       </c>
-      <c r="D48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="n">
+        <v>-107</v>
+      </c>
       <c r="E48" t="n">
-        <v>-107</v>
+        <v>24</v>
       </c>
       <c r="F48" t="n">
-        <v>24</v>
-      </c>
-      <c r="G48" t="n">
         <v>18</v>
       </c>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="n">
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="n">
         <v>-104</v>
       </c>
     </row>
@@ -1780,23 +1652,20 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>19</v>
-      </c>
-      <c r="C49" t="n">
-        <v>25</v>
-      </c>
-      <c r="D49" t="inlineStr"/>
+        <v>25</v>
+      </c>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="n">
+        <v>-111</v>
+      </c>
       <c r="E49" t="n">
-        <v>-111</v>
+        <v>-103</v>
       </c>
       <c r="F49" t="n">
-        <v>-103</v>
-      </c>
-      <c r="G49" t="n">
         <v>17</v>
       </c>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="n">
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1807,21 +1676,18 @@
       <c r="B50" t="n">
         <v>25</v>
       </c>
-      <c r="C50" t="n">
-        <v>25</v>
-      </c>
-      <c r="D50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="n">
+        <v>-119</v>
+      </c>
       <c r="E50" t="n">
-        <v>-119</v>
+        <v>-104</v>
       </c>
       <c r="F50" t="n">
-        <v>-104</v>
-      </c>
-      <c r="G50" t="n">
         <v>17</v>
       </c>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="n">
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1832,21 +1698,18 @@
       <c r="B51" t="n">
         <v>25</v>
       </c>
-      <c r="C51" t="n">
-        <v>25</v>
-      </c>
-      <c r="D51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="n">
+        <v>-109</v>
+      </c>
       <c r="E51" t="n">
-        <v>-109</v>
+        <v>-104</v>
       </c>
       <c r="F51" t="n">
-        <v>-104</v>
-      </c>
-      <c r="G51" t="n">
         <v>15</v>
       </c>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="n">
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="n">
         <v>-103</v>
       </c>
     </row>
@@ -1857,21 +1720,18 @@
       <c r="B52" t="n">
         <v>25</v>
       </c>
-      <c r="C52" t="n">
-        <v>25</v>
-      </c>
-      <c r="D52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="n">
+        <v>-107</v>
+      </c>
       <c r="E52" t="n">
-        <v>-107</v>
+        <v>25</v>
       </c>
       <c r="F52" t="n">
-        <v>25</v>
-      </c>
-      <c r="G52" t="n">
         <v>16</v>
       </c>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="n">
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1880,23 +1740,20 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>25</v>
-      </c>
-      <c r="C53" t="n">
         <v>-103</v>
       </c>
-      <c r="D53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="n">
+        <v>-107</v>
+      </c>
       <c r="E53" t="n">
-        <v>-107</v>
+        <v>-105</v>
       </c>
       <c r="F53" t="n">
-        <v>-105</v>
-      </c>
-      <c r="G53" t="n">
         <v>17</v>
       </c>
+      <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -1905,90 +1762,78 @@
       <c r="B54" t="n">
         <v>25</v>
       </c>
-      <c r="C54" t="n">
-        <v>25</v>
-      </c>
-      <c r="D54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="n">
+        <v>-107</v>
+      </c>
       <c r="E54" t="n">
-        <v>-107</v>
+        <v>-109</v>
       </c>
       <c r="F54" t="n">
-        <v>-109</v>
-      </c>
-      <c r="G54" t="n">
         <v>2</v>
       </c>
+      <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>12</v>
-      </c>
-      <c r="C55" t="n">
-        <v>25</v>
-      </c>
-      <c r="D55" t="inlineStr"/>
+        <v>25</v>
+      </c>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="n">
+        <v>-107</v>
+      </c>
       <c r="E55" t="n">
-        <v>-107</v>
+        <v>24</v>
       </c>
       <c r="F55" t="n">
-        <v>24</v>
-      </c>
-      <c r="G55" t="n">
         <v>20</v>
       </c>
+      <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>24</v>
-      </c>
-      <c r="C56" t="n">
-        <v>25</v>
-      </c>
-      <c r="D56" t="inlineStr"/>
+        <v>25</v>
+      </c>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="n">
+        <v>-107</v>
+      </c>
       <c r="E56" t="n">
-        <v>-107</v>
+        <v>-104</v>
       </c>
       <c r="F56" t="n">
-        <v>-104</v>
-      </c>
-      <c r="G56" t="n">
         <v>-124</v>
       </c>
+      <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-110</v>
-      </c>
-      <c r="C57" t="n">
-        <v>25</v>
-      </c>
-      <c r="D57" t="inlineStr"/>
+        <v>25</v>
+      </c>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="n">
+        <v>-107</v>
+      </c>
       <c r="E57" t="n">
-        <v>-107</v>
+        <v>-104</v>
       </c>
       <c r="F57" t="n">
-        <v>-104</v>
-      </c>
-      <c r="G57" t="n">
         <v>-113</v>
       </c>
+      <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -1997,21 +1842,18 @@
       <c r="B58" t="n">
         <v>25</v>
       </c>
-      <c r="C58" t="n">
-        <v>25</v>
-      </c>
-      <c r="D58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="n">
+        <v>-107</v>
+      </c>
       <c r="E58" t="n">
-        <v>-107</v>
+        <v>24</v>
       </c>
       <c r="F58" t="n">
-        <v>24</v>
-      </c>
-      <c r="G58" t="n">
         <v>-113</v>
       </c>
+      <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -2020,21 +1862,18 @@
       <c r="B59" t="n">
         <v>25</v>
       </c>
-      <c r="C59" t="n">
-        <v>25</v>
-      </c>
-      <c r="D59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="n">
+        <v>-110</v>
+      </c>
       <c r="E59" t="n">
-        <v>-110</v>
+        <v>24</v>
       </c>
       <c r="F59" t="n">
-        <v>24</v>
-      </c>
-      <c r="G59" t="n">
         <v>22</v>
       </c>
+      <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -2043,99 +1882,98 @@
       <c r="B60" t="n">
         <v>25</v>
       </c>
-      <c r="C60" t="n">
-        <v>25</v>
-      </c>
-      <c r="D60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="n">
+        <v>16</v>
+      </c>
       <c r="E60" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F60" t="n">
-        <v>24</v>
-      </c>
-      <c r="G60" t="n">
         <v>20</v>
       </c>
+      <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>20</v>
+        <v>-107</v>
       </c>
       <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
+      <c r="D61" t="n">
+        <v>-107</v>
+      </c>
       <c r="E61" t="n">
-        <v>-107</v>
+        <v>-105</v>
       </c>
       <c r="F61" t="n">
-        <v>-105</v>
-      </c>
-      <c r="G61" t="n">
         <v>14</v>
       </c>
+      <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B62" t="inlineStr"/>
+      <c r="B62" t="n">
+        <v>-106</v>
+      </c>
       <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
+      <c r="D62" t="n">
+        <v>-110</v>
+      </c>
       <c r="E62" t="n">
-        <v>-110</v>
+        <v>-103</v>
       </c>
       <c r="F62" t="n">
-        <v>-103</v>
-      </c>
-      <c r="G62" t="n">
         <v>20</v>
       </c>
+      <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
-      <c r="I62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B63" t="inlineStr"/>
+      <c r="B63" t="n">
+        <v>-104</v>
+      </c>
       <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
+      <c r="D63" t="n">
+        <v>21</v>
+      </c>
       <c r="E63" t="n">
+        <v>-109</v>
+      </c>
+      <c r="F63" t="n">
         <v>21</v>
       </c>
-      <c r="F63" t="n">
-        <v>-109</v>
-      </c>
-      <c r="G63" t="n">
-        <v>21</v>
-      </c>
+      <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B64" t="inlineStr"/>
+      <c r="B64" t="n">
+        <v>25</v>
+      </c>
       <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
+      <c r="D64" t="n">
+        <v>-107</v>
+      </c>
       <c r="E64" t="n">
-        <v>-107</v>
+        <v>24</v>
       </c>
       <c r="F64" t="n">
-        <v>24</v>
-      </c>
-      <c r="G64" t="n">
         <v>15</v>
       </c>
+      <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
-      <c r="I64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -2143,18 +1981,17 @@
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr"/>
+      <c r="D65" t="n">
+        <v>-107</v>
+      </c>
       <c r="E65" t="n">
+        <v>24</v>
+      </c>
+      <c r="F65" t="n">
         <v>-107</v>
       </c>
-      <c r="F65" t="n">
-        <v>24</v>
-      </c>
-      <c r="G65" t="n">
-        <v>-107</v>
-      </c>
+      <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -2162,18 +1999,17 @@
       </c>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr"/>
+      <c r="D66" t="n">
+        <v>-107</v>
+      </c>
       <c r="E66" t="n">
-        <v>-107</v>
+        <v>-105</v>
       </c>
       <c r="F66" t="n">
-        <v>-105</v>
-      </c>
-      <c r="G66" t="n">
         <v>20</v>
       </c>
+      <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
-      <c r="I66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -2181,18 +2017,17 @@
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr"/>
+      <c r="D67" t="n">
+        <v>5</v>
+      </c>
       <c r="E67" t="n">
-        <v>5</v>
+        <v>-105</v>
       </c>
       <c r="F67" t="n">
-        <v>-105</v>
-      </c>
-      <c r="G67" t="n">
         <v>-137</v>
       </c>
+      <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
-      <c r="I67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -2200,16 +2035,17 @@
       </c>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr"/>
+      <c r="D68" t="n">
+        <v>-112</v>
+      </c>
+      <c r="E68" t="n">
+        <v>24</v>
+      </c>
       <c r="F68" t="n">
-        <v>24</v>
-      </c>
-      <c r="G68" t="n">
         <v>17</v>
       </c>
+      <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
-      <c r="I68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -2217,16 +2053,17 @@
       </c>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr"/>
+      <c r="D69" t="n">
+        <v>-104</v>
+      </c>
+      <c r="E69" t="n">
+        <v>24</v>
+      </c>
       <c r="F69" t="n">
-        <v>24</v>
-      </c>
-      <c r="G69" t="n">
         <v>-136</v>
       </c>
+      <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
-      <c r="I69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -2234,16 +2071,17 @@
       </c>
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr"/>
+      <c r="D70" t="n">
+        <v>-8</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-104</v>
+      </c>
       <c r="F70" t="n">
-        <v>-104</v>
-      </c>
-      <c r="G70" t="n">
         <v>17</v>
       </c>
+      <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr"/>
-      <c r="I70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -2251,16 +2089,17 @@
       </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr"/>
+      <c r="D71" t="n">
+        <v>21</v>
+      </c>
+      <c r="E71" t="n">
+        <v>24</v>
+      </c>
       <c r="F71" t="n">
-        <v>24</v>
-      </c>
-      <c r="G71" t="n">
         <v>12</v>
       </c>
+      <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
-      <c r="I71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -2269,15 +2108,14 @@
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr"/>
+      <c r="E72" t="n">
+        <v>-107</v>
+      </c>
       <c r="F72" t="n">
-        <v>-107</v>
-      </c>
-      <c r="G72" t="n">
         <v>-106</v>
       </c>
+      <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
-      <c r="I72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -2286,15 +2124,14 @@
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr"/>
+      <c r="E73" t="n">
+        <v>24</v>
+      </c>
       <c r="F73" t="n">
-        <v>24</v>
-      </c>
-      <c r="G73" t="n">
         <v>9</v>
       </c>
+      <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
-      <c r="I73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -2303,15 +2140,14 @@
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr"/>
+      <c r="E74" t="n">
+        <v>-105</v>
+      </c>
       <c r="F74" t="n">
-        <v>-105</v>
-      </c>
-      <c r="G74" t="n">
         <v>20</v>
       </c>
+      <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
-      <c r="I74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -2320,15 +2156,14 @@
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
+      <c r="E75" t="n">
+        <v>24</v>
+      </c>
       <c r="F75" t="n">
-        <v>24</v>
-      </c>
-      <c r="G75" t="n">
         <v>-111</v>
       </c>
+      <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
-      <c r="I75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -2337,15 +2172,14 @@
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr"/>
+      <c r="E76" t="n">
+        <v>-104</v>
+      </c>
       <c r="F76" t="n">
-        <v>-104</v>
-      </c>
-      <c r="G76" t="n">
         <v>19</v>
       </c>
+      <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
-      <c r="I76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -2354,15 +2188,14 @@
       <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr"/>
+      <c r="E77" t="n">
+        <v>-107</v>
+      </c>
       <c r="F77" t="n">
-        <v>-107</v>
-      </c>
-      <c r="G77" t="n">
         <v>17</v>
       </c>
+      <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
-      <c r="I77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -2371,15 +2204,72 @@
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
+      <c r="E78" t="n">
+        <v>-104</v>
+      </c>
       <c r="F78" t="n">
-        <v>-104</v>
-      </c>
-      <c r="G78" t="n">
         <v>17</v>
       </c>
+      <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
-      <c r="I78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="n">
+        <v>-105</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-110</v>
+      </c>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="n">
+        <v>-102</v>
+      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
+      <c r="E81" t="n">
+        <v>-107</v>
+      </c>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="n">
+        <v>-105</v>
+      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2392,7 +2282,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2403,40 +2293,35 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Social VI</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>aggressiveBehavior</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>carefulBehavior</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>randomBehavior</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>semiAggressiveBehavior</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>semiCarefulBehavior</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>valueIterationBasedBehavior_v2</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>valueIterationBasedBehavior_v2.1</t>
         </is>
@@ -2447,27 +2332,24 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
+        <v>-210</v>
+      </c>
+      <c r="C2" t="n">
         <v>43</v>
       </c>
-      <c r="C2" t="n">
-        <v>-210</v>
-      </c>
       <c r="D2" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" t="n">
-        <v>40</v>
+        <v>-206</v>
       </c>
       <c r="F2" t="n">
+        <v>17</v>
+      </c>
+      <c r="G2" t="n">
         <v>-206</v>
       </c>
-      <c r="G2" t="n">
-        <v>17</v>
-      </c>
       <c r="H2" t="n">
-        <v>-206</v>
-      </c>
-      <c r="I2" t="n">
         <v>46</v>
       </c>
     </row>
@@ -2476,27 +2358,24 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>-206</v>
+        <v>46</v>
       </c>
       <c r="C3" t="n">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D3" t="n">
-        <v>41</v>
+        <v>-210</v>
       </c>
       <c r="E3" t="n">
-        <v>-210</v>
+        <v>-208</v>
       </c>
       <c r="F3" t="n">
-        <v>-208</v>
+        <v>43</v>
       </c>
       <c r="G3" t="n">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H3" t="n">
-        <v>48</v>
-      </c>
-      <c r="I3" t="n">
         <v>39</v>
       </c>
     </row>
@@ -2505,27 +2384,24 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
+        <v>-210</v>
+      </c>
+      <c r="C4" t="n">
+        <v>43</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-270</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-206</v>
+      </c>
+      <c r="F4" t="n">
         <v>39</v>
       </c>
-      <c r="C4" t="n">
-        <v>-210</v>
-      </c>
-      <c r="D4" t="n">
-        <v>43</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-270</v>
-      </c>
-      <c r="F4" t="n">
-        <v>-206</v>
-      </c>
       <c r="G4" t="n">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="H4" t="n">
-        <v>48</v>
-      </c>
-      <c r="I4" t="n">
         <v>47</v>
       </c>
     </row>
@@ -2534,27 +2410,24 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="C5" t="n">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D5" t="n">
-        <v>43</v>
+        <v>-220</v>
       </c>
       <c r="E5" t="n">
-        <v>-220</v>
+        <v>-210</v>
       </c>
       <c r="F5" t="n">
-        <v>-210</v>
+        <v>23</v>
       </c>
       <c r="G5" t="n">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="H5" t="n">
-        <v>47</v>
-      </c>
-      <c r="I5" t="n">
         <v>-206</v>
       </c>
     </row>
@@ -2563,27 +2436,24 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>45</v>
+        <v>-210</v>
       </c>
       <c r="C6" t="n">
-        <v>-210</v>
+        <v>40</v>
       </c>
       <c r="D6" t="n">
-        <v>40</v>
+        <v>-208</v>
       </c>
       <c r="E6" t="n">
-        <v>-208</v>
+        <v>43</v>
       </c>
       <c r="F6" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G6" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="H6" t="n">
-        <v>47</v>
-      </c>
-      <c r="I6" t="n">
         <v>44</v>
       </c>
     </row>
@@ -2592,27 +2462,24 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>26</v>
+        <v>-214</v>
       </c>
       <c r="C7" t="n">
+        <v>43</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-222</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-210</v>
+      </c>
+      <c r="F7" t="n">
+        <v>36</v>
+      </c>
+      <c r="G7" t="n">
         <v>-214</v>
       </c>
-      <c r="D7" t="n">
-        <v>43</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-222</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-210</v>
-      </c>
-      <c r="G7" t="n">
-        <v>36</v>
-      </c>
       <c r="H7" t="n">
-        <v>-214</v>
-      </c>
-      <c r="I7" t="n">
         <v>-208</v>
       </c>
     </row>
@@ -2621,27 +2488,24 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" t="n">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D8" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E8" t="n">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F8" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G8" t="n">
-        <v>40</v>
+        <v>-216</v>
       </c>
       <c r="H8" t="n">
-        <v>-216</v>
-      </c>
-      <c r="I8" t="n">
         <v>48</v>
       </c>
     </row>
@@ -2650,27 +2514,24 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>48</v>
+        <v>-208</v>
       </c>
       <c r="C9" t="n">
+        <v>47</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-232</v>
+      </c>
+      <c r="E9" t="n">
         <v>-208</v>
       </c>
-      <c r="D9" t="n">
-        <v>47</v>
-      </c>
-      <c r="E9" t="n">
-        <v>-232</v>
-      </c>
       <c r="F9" t="n">
-        <v>-208</v>
+        <v>31</v>
       </c>
       <c r="G9" t="n">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="H9" t="n">
-        <v>47</v>
-      </c>
-      <c r="I9" t="n">
         <v>45</v>
       </c>
     </row>
@@ -2679,27 +2540,24 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="C10" t="n">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D10" t="n">
-        <v>43</v>
+        <v>-210</v>
       </c>
       <c r="E10" t="n">
-        <v>-210</v>
+        <v>-206</v>
       </c>
       <c r="F10" t="n">
+        <v>-266</v>
+      </c>
+      <c r="G10" t="n">
         <v>-206</v>
       </c>
-      <c r="G10" t="n">
-        <v>-266</v>
-      </c>
       <c r="H10" t="n">
-        <v>-206</v>
-      </c>
-      <c r="I10" t="n">
         <v>-208</v>
       </c>
     </row>
@@ -2708,27 +2566,24 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" t="n">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D11" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E11" t="n">
-        <v>45</v>
+        <v>-208</v>
       </c>
       <c r="F11" t="n">
         <v>-208</v>
       </c>
       <c r="G11" t="n">
-        <v>-208</v>
+        <v>48</v>
       </c>
       <c r="H11" t="n">
-        <v>48</v>
-      </c>
-      <c r="I11" t="n">
         <v>48</v>
       </c>
     </row>
@@ -2740,24 +2595,21 @@
         <v>48</v>
       </c>
       <c r="C12" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D12" t="n">
-        <v>24</v>
+        <v>-218</v>
       </c>
       <c r="E12" t="n">
-        <v>-218</v>
+        <v>-210</v>
       </c>
       <c r="F12" t="n">
-        <v>-210</v>
+        <v>39</v>
       </c>
       <c r="G12" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="H12" t="n">
-        <v>33</v>
-      </c>
-      <c r="I12" t="n">
         <v>47</v>
       </c>
     </row>
@@ -2766,27 +2618,24 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>-206</v>
+        <v>-208</v>
       </c>
       <c r="C13" t="n">
-        <v>-208</v>
+        <v>43</v>
       </c>
       <c r="D13" t="n">
+        <v>-220</v>
+      </c>
+      <c r="E13" t="n">
+        <v>45</v>
+      </c>
+      <c r="F13" t="n">
+        <v>15</v>
+      </c>
+      <c r="G13" t="n">
         <v>43</v>
       </c>
-      <c r="E13" t="n">
-        <v>-220</v>
-      </c>
-      <c r="F13" t="n">
-        <v>45</v>
-      </c>
-      <c r="G13" t="n">
-        <v>15</v>
-      </c>
       <c r="H13" t="n">
-        <v>43</v>
-      </c>
-      <c r="I13" t="n">
         <v>48</v>
       </c>
     </row>
@@ -2795,27 +2644,24 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>-206</v>
+        <v>46</v>
       </c>
       <c r="C14" t="n">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D14" t="n">
-        <v>43</v>
+        <v>-210</v>
       </c>
       <c r="E14" t="n">
-        <v>-210</v>
+        <v>-208</v>
       </c>
       <c r="F14" t="n">
-        <v>-208</v>
+        <v>39</v>
       </c>
       <c r="G14" t="n">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H14" t="n">
-        <v>47</v>
-      </c>
-      <c r="I14" t="n">
         <v>48</v>
       </c>
     </row>
@@ -2824,27 +2670,24 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>39</v>
+        <v>-206</v>
       </c>
       <c r="C15" t="n">
+        <v>43</v>
+      </c>
+      <c r="D15" t="n">
         <v>-206</v>
       </c>
-      <c r="D15" t="n">
-        <v>43</v>
-      </c>
       <c r="E15" t="n">
-        <v>-206</v>
+        <v>-216</v>
       </c>
       <c r="F15" t="n">
-        <v>-216</v>
+        <v>33</v>
       </c>
       <c r="G15" t="n">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="H15" t="n">
-        <v>23</v>
-      </c>
-      <c r="I15" t="n">
         <v>48</v>
       </c>
     </row>
@@ -2853,27 +2696,24 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>-206</v>
+        <v>47</v>
       </c>
       <c r="C16" t="n">
         <v>47</v>
       </c>
       <c r="D16" t="n">
-        <v>47</v>
+        <v>-220</v>
       </c>
       <c r="E16" t="n">
-        <v>-220</v>
+        <v>43</v>
       </c>
       <c r="F16" t="n">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G16" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H16" t="n">
-        <v>49</v>
-      </c>
-      <c r="I16" t="n">
         <v>-250</v>
       </c>
     </row>
@@ -2882,27 +2722,24 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C17" t="n">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D17" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E17" t="n">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F17" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G17" t="n">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="H17" t="n">
-        <v>49</v>
-      </c>
-      <c r="I17" t="n">
         <v>45</v>
       </c>
     </row>
@@ -2914,24 +2751,21 @@
         <v>47</v>
       </c>
       <c r="C18" t="n">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D18" t="n">
-        <v>33</v>
+        <v>-216</v>
       </c>
       <c r="E18" t="n">
-        <v>-216</v>
+        <v>-210</v>
       </c>
       <c r="F18" t="n">
-        <v>-210</v>
+        <v>39</v>
       </c>
       <c r="G18" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H18" t="n">
-        <v>43</v>
-      </c>
-      <c r="I18" t="n">
         <v>-206</v>
       </c>
     </row>
@@ -2940,27 +2774,24 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>-3</v>
+        <v>-206</v>
       </c>
       <c r="C19" t="n">
-        <v>-206</v>
+        <v>40</v>
       </c>
       <c r="D19" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="E19" t="n">
-        <v>30</v>
+        <v>-228</v>
       </c>
       <c r="F19" t="n">
-        <v>-228</v>
+        <v>32</v>
       </c>
       <c r="G19" t="n">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="H19" t="n">
-        <v>41</v>
-      </c>
-      <c r="I19" t="n">
         <v>46</v>
       </c>
     </row>
@@ -2969,27 +2800,24 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" t="n">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D20" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E20" t="n">
-        <v>46</v>
+        <v>-210</v>
       </c>
       <c r="F20" t="n">
-        <v>-210</v>
+        <v>33</v>
       </c>
       <c r="G20" t="n">
-        <v>33</v>
+        <v>-218</v>
       </c>
       <c r="H20" t="n">
-        <v>-218</v>
-      </c>
-      <c r="I20" t="n">
         <v>-268</v>
       </c>
     </row>
@@ -2998,27 +2826,24 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>-206</v>
+        <v>-208</v>
       </c>
       <c r="C21" t="n">
-        <v>-208</v>
+        <v>43</v>
       </c>
       <c r="D21" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" t="n">
-        <v>42</v>
+        <v>-210</v>
       </c>
       <c r="F21" t="n">
-        <v>-210</v>
+        <v>45</v>
       </c>
       <c r="G21" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H21" t="n">
-        <v>48</v>
-      </c>
-      <c r="I21" t="n">
         <v>-208</v>
       </c>
     </row>
@@ -3027,27 +2852,24 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>47</v>
+        <v>-206</v>
       </c>
       <c r="C22" t="n">
-        <v>-206</v>
+        <v>43</v>
       </c>
       <c r="D22" t="n">
-        <v>43</v>
+        <v>-212</v>
       </c>
       <c r="E22" t="n">
-        <v>-212</v>
+        <v>45</v>
       </c>
       <c r="F22" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G22" t="n">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="H22" t="n">
-        <v>40</v>
-      </c>
-      <c r="I22" t="n">
         <v>45</v>
       </c>
     </row>
@@ -3059,24 +2881,21 @@
         <v>48</v>
       </c>
       <c r="C23" t="n">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D23" t="n">
-        <v>43</v>
+        <v>-226</v>
       </c>
       <c r="E23" t="n">
-        <v>-226</v>
+        <v>45</v>
       </c>
       <c r="F23" t="n">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G23" t="n">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="H23" t="n">
-        <v>31</v>
-      </c>
-      <c r="I23" t="n">
         <v>-206</v>
       </c>
     </row>
@@ -3085,27 +2904,24 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" t="n">
         <v>47</v>
       </c>
       <c r="D24" t="n">
-        <v>47</v>
+        <v>-210</v>
       </c>
       <c r="E24" t="n">
-        <v>-210</v>
+        <v>-208</v>
       </c>
       <c r="F24" t="n">
-        <v>-208</v>
+        <v>37</v>
       </c>
       <c r="G24" t="n">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="H24" t="n">
-        <v>44</v>
-      </c>
-      <c r="I24" t="n">
         <v>48</v>
       </c>
     </row>
@@ -3114,27 +2930,24 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>29</v>
+        <v>-206</v>
       </c>
       <c r="C25" t="n">
-        <v>-206</v>
+        <v>43</v>
       </c>
       <c r="D25" t="n">
-        <v>43</v>
+        <v>-208</v>
       </c>
       <c r="E25" t="n">
-        <v>-208</v>
+        <v>45</v>
       </c>
       <c r="F25" t="n">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="G25" t="n">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="H25" t="n">
-        <v>47</v>
-      </c>
-      <c r="I25" t="n">
         <v>48</v>
       </c>
     </row>
@@ -3143,27 +2956,24 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C26" t="n">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D26" t="n">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E26" t="n">
-        <v>39</v>
+        <v>-210</v>
       </c>
       <c r="F26" t="n">
         <v>-210</v>
       </c>
       <c r="G26" t="n">
-        <v>-210</v>
+        <v>48</v>
       </c>
       <c r="H26" t="n">
-        <v>48</v>
-      </c>
-      <c r="I26" t="n">
         <v>47</v>
       </c>
     </row>
@@ -3175,24 +2985,21 @@
         <v>-206</v>
       </c>
       <c r="C27" t="n">
-        <v>-206</v>
+        <v>47</v>
       </c>
       <c r="D27" t="n">
-        <v>47</v>
+        <v>-210</v>
       </c>
       <c r="E27" t="n">
-        <v>-210</v>
+        <v>-208</v>
       </c>
       <c r="F27" t="n">
-        <v>-208</v>
+        <v>36</v>
       </c>
       <c r="G27" t="n">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="H27" t="n">
-        <v>23</v>
-      </c>
-      <c r="I27" t="n">
         <v>48</v>
       </c>
     </row>
@@ -3201,27 +3008,24 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C28" t="n">
+        <v>43</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-212</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-226</v>
+      </c>
+      <c r="F28" t="n">
+        <v>33</v>
+      </c>
+      <c r="G28" t="n">
         <v>48</v>
       </c>
-      <c r="D28" t="n">
-        <v>43</v>
-      </c>
-      <c r="E28" t="n">
-        <v>-212</v>
-      </c>
-      <c r="F28" t="n">
-        <v>-226</v>
-      </c>
-      <c r="G28" t="n">
-        <v>33</v>
-      </c>
       <c r="H28" t="n">
-        <v>48</v>
-      </c>
-      <c r="I28" t="n">
         <v>48</v>
       </c>
     </row>
@@ -3230,27 +3034,24 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C29" t="n">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D29" t="n">
-        <v>39</v>
+        <v>-244</v>
       </c>
       <c r="E29" t="n">
-        <v>-244</v>
+        <v>45</v>
       </c>
       <c r="F29" t="n">
+        <v>43</v>
+      </c>
+      <c r="G29" t="n">
         <v>45</v>
       </c>
-      <c r="G29" t="n">
-        <v>43</v>
-      </c>
       <c r="H29" t="n">
-        <v>45</v>
-      </c>
-      <c r="I29" t="n">
         <v>47</v>
       </c>
     </row>
@@ -3259,25 +3060,24 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C30" t="n">
-        <v>47</v>
-      </c>
-      <c r="D30" t="inlineStr"/>
+        <v>-236</v>
+      </c>
+      <c r="D30" t="n">
+        <v>-210</v>
+      </c>
       <c r="E30" t="n">
-        <v>-210</v>
+        <v>-208</v>
       </c>
       <c r="F30" t="n">
-        <v>-208</v>
+        <v>13</v>
       </c>
       <c r="G30" t="n">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="H30" t="n">
-        <v>43</v>
-      </c>
-      <c r="I30" t="n">
         <v>45</v>
       </c>
     </row>
@@ -3289,22 +3089,21 @@
         <v>47</v>
       </c>
       <c r="C31" t="n">
-        <v>47</v>
-      </c>
-      <c r="D31" t="inlineStr"/>
+        <v>-208</v>
+      </c>
+      <c r="D31" t="n">
+        <v>-210</v>
+      </c>
       <c r="E31" t="n">
-        <v>-210</v>
+        <v>-208</v>
       </c>
       <c r="F31" t="n">
-        <v>-208</v>
+        <v>43</v>
       </c>
       <c r="G31" t="n">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="H31" t="n">
-        <v>48</v>
-      </c>
-      <c r="I31" t="n">
         <v>46</v>
       </c>
     </row>
@@ -3313,25 +3112,24 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>-206</v>
+        <v>-210</v>
       </c>
       <c r="C32" t="n">
-        <v>-210</v>
-      </c>
-      <c r="D32" t="inlineStr"/>
+        <v>43</v>
+      </c>
+      <c r="D32" t="n">
+        <v>-214</v>
+      </c>
       <c r="E32" t="n">
-        <v>-214</v>
+        <v>43</v>
       </c>
       <c r="F32" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G32" t="n">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="H32" t="n">
-        <v>28</v>
-      </c>
-      <c r="I32" t="n">
         <v>-206</v>
       </c>
     </row>
@@ -3340,25 +3138,24 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>-3</v>
+        <v>-206</v>
       </c>
       <c r="C33" t="n">
+        <v>43</v>
+      </c>
+      <c r="D33" t="n">
+        <v>-214</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-208</v>
+      </c>
+      <c r="F33" t="n">
+        <v>43</v>
+      </c>
+      <c r="G33" t="n">
         <v>-206</v>
       </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="n">
-        <v>-214</v>
-      </c>
-      <c r="F33" t="n">
-        <v>-208</v>
-      </c>
-      <c r="G33" t="n">
-        <v>43</v>
-      </c>
       <c r="H33" t="n">
-        <v>-206</v>
-      </c>
-      <c r="I33" t="n">
         <v>-224</v>
       </c>
     </row>
@@ -3367,25 +3164,24 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C34" t="n">
         <v>47</v>
       </c>
-      <c r="D34" t="inlineStr"/>
+      <c r="D34" t="n">
+        <v>-304</v>
+      </c>
       <c r="E34" t="n">
-        <v>-304</v>
+        <v>-208</v>
       </c>
       <c r="F34" t="n">
-        <v>-208</v>
+        <v>37</v>
       </c>
       <c r="G34" t="n">
         <v>37</v>
       </c>
       <c r="H34" t="n">
-        <v>37</v>
-      </c>
-      <c r="I34" t="n">
         <v>47</v>
       </c>
     </row>
@@ -3396,23 +3192,20 @@
       <c r="B35" t="n">
         <v>47</v>
       </c>
-      <c r="C35" t="n">
-        <v>47</v>
-      </c>
-      <c r="D35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="n">
+        <v>46</v>
+      </c>
       <c r="E35" t="n">
-        <v>46</v>
+        <v>-208</v>
       </c>
       <c r="F35" t="n">
-        <v>-208</v>
+        <v>47</v>
       </c>
       <c r="G35" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H35" t="n">
-        <v>44</v>
-      </c>
-      <c r="I35" t="n">
         <v>47</v>
       </c>
     </row>
@@ -3423,21 +3216,20 @@
       <c r="B36" t="n">
         <v>48</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="n">
+        <v>42</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-210</v>
+      </c>
+      <c r="F36" t="n">
+        <v>29</v>
+      </c>
+      <c r="G36" t="n">
         <v>48</v>
       </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="n">
-        <v>42</v>
-      </c>
-      <c r="F36" t="n">
-        <v>-210</v>
-      </c>
-      <c r="G36" t="n">
-        <v>29</v>
-      </c>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="n">
+      <c r="H36" t="n">
         <v>46</v>
       </c>
     </row>
@@ -3446,23 +3238,22 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>31</v>
-      </c>
-      <c r="C37" t="n">
         <v>48</v>
       </c>
-      <c r="D37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="n">
+        <v>30</v>
+      </c>
       <c r="E37" t="n">
-        <v>30</v>
+        <v>-206</v>
       </c>
       <c r="F37" t="n">
-        <v>-206</v>
+        <v>47</v>
       </c>
       <c r="G37" t="n">
         <v>47</v>
       </c>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="n">
+      <c r="H37" t="n">
         <v>46</v>
       </c>
     </row>
@@ -3471,23 +3262,22 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>47</v>
-      </c>
-      <c r="C38" t="n">
         <v>-206</v>
       </c>
-      <c r="D38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="n">
+        <v>46</v>
+      </c>
       <c r="E38" t="n">
-        <v>46</v>
+        <v>-208</v>
       </c>
       <c r="F38" t="n">
+        <v>41</v>
+      </c>
+      <c r="G38" t="n">
         <v>-208</v>
       </c>
-      <c r="G38" t="n">
-        <v>41</v>
-      </c>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="n">
+      <c r="H38" t="n">
         <v>48</v>
       </c>
     </row>
@@ -3496,23 +3286,22 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>48</v>
-      </c>
-      <c r="C39" t="n">
         <v>36</v>
       </c>
-      <c r="D39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="n">
+        <v>-292</v>
+      </c>
       <c r="E39" t="n">
-        <v>-292</v>
+        <v>45</v>
       </c>
       <c r="F39" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G39" t="n">
-        <v>37</v>
-      </c>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="n">
+        <v>-290</v>
+      </c>
+      <c r="H39" t="n">
         <v>-206</v>
       </c>
     </row>
@@ -3521,23 +3310,20 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>46</v>
-      </c>
-      <c r="C40" t="n">
-        <v>47</v>
-      </c>
-      <c r="D40" t="inlineStr"/>
+        <v>47</v>
+      </c>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="n">
+        <v>-222</v>
+      </c>
       <c r="E40" t="n">
-        <v>-222</v>
+        <v>-208</v>
       </c>
       <c r="F40" t="n">
-        <v>-208</v>
-      </c>
-      <c r="G40" t="n">
         <v>42</v>
       </c>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="n">
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="n">
         <v>47</v>
       </c>
     </row>
@@ -3546,23 +3332,20 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>48</v>
-      </c>
-      <c r="C41" t="n">
-        <v>47</v>
-      </c>
-      <c r="D41" t="inlineStr"/>
+        <v>47</v>
+      </c>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="n">
+        <v>-218</v>
+      </c>
       <c r="E41" t="n">
-        <v>-218</v>
+        <v>45</v>
       </c>
       <c r="F41" t="n">
-        <v>45</v>
-      </c>
-      <c r="G41" t="n">
         <v>41</v>
       </c>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="n">
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="n">
         <v>47</v>
       </c>
     </row>
@@ -3571,23 +3354,20 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>-214</v>
-      </c>
-      <c r="C42" t="n">
         <v>-206</v>
       </c>
-      <c r="D42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="n">
+        <v>30</v>
+      </c>
       <c r="E42" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="F42" t="n">
-        <v>45</v>
-      </c>
-      <c r="G42" t="n">
-        <v>25</v>
-      </c>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="n">
+        <v>25</v>
+      </c>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="n">
         <v>22</v>
       </c>
     </row>
@@ -3596,23 +3376,20 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>43</v>
-      </c>
-      <c r="C43" t="n">
-        <v>47</v>
-      </c>
-      <c r="D43" t="inlineStr"/>
+        <v>47</v>
+      </c>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="n">
+        <v>46</v>
+      </c>
       <c r="E43" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F43" t="n">
-        <v>45</v>
-      </c>
-      <c r="G43" t="n">
         <v>30</v>
       </c>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="n">
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="n">
         <v>45</v>
       </c>
     </row>
@@ -3621,23 +3398,20 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>-206</v>
-      </c>
-      <c r="C44" t="n">
-        <v>47</v>
-      </c>
-      <c r="D44" t="inlineStr"/>
+        <v>47</v>
+      </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="n">
+        <v>-214</v>
+      </c>
       <c r="E44" t="n">
-        <v>-214</v>
+        <v>-210</v>
       </c>
       <c r="F44" t="n">
-        <v>-210</v>
-      </c>
-      <c r="G44" t="n">
         <v>18</v>
       </c>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="n">
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="n">
         <v>48</v>
       </c>
     </row>
@@ -3646,23 +3420,20 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>48</v>
-      </c>
-      <c r="C45" t="n">
         <v>44</v>
       </c>
-      <c r="D45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="n">
+        <v>-214</v>
+      </c>
       <c r="E45" t="n">
-        <v>-214</v>
+        <v>-206</v>
       </c>
       <c r="F45" t="n">
-        <v>-206</v>
-      </c>
-      <c r="G45" t="n">
         <v>43</v>
       </c>
-      <c r="H45" t="inlineStr"/>
-      <c r="I45" t="n">
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="n">
         <v>-216</v>
       </c>
     </row>
@@ -3671,23 +3442,20 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>45</v>
-      </c>
-      <c r="C46" t="n">
         <v>46</v>
       </c>
-      <c r="D46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="n">
+        <v>-222</v>
+      </c>
       <c r="E46" t="n">
-        <v>-222</v>
+        <v>-208</v>
       </c>
       <c r="F46" t="n">
-        <v>-208</v>
-      </c>
-      <c r="G46" t="n">
         <v>41</v>
       </c>
-      <c r="H46" t="inlineStr"/>
-      <c r="I46" t="n">
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="n">
         <v>47</v>
       </c>
     </row>
@@ -3698,21 +3466,18 @@
       <c r="B47" t="n">
         <v>47</v>
       </c>
-      <c r="C47" t="n">
-        <v>47</v>
-      </c>
-      <c r="D47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="n">
+        <v>-224</v>
+      </c>
       <c r="E47" t="n">
-        <v>-224</v>
+        <v>-210</v>
       </c>
       <c r="F47" t="n">
-        <v>-210</v>
-      </c>
-      <c r="G47" t="n">
         <v>29</v>
       </c>
-      <c r="H47" t="inlineStr"/>
-      <c r="I47" t="n">
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="n">
         <v>-206</v>
       </c>
     </row>
@@ -3721,23 +3486,20 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>47</v>
-      </c>
-      <c r="C48" t="n">
         <v>-216</v>
       </c>
-      <c r="D48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="n">
+        <v>-214</v>
+      </c>
       <c r="E48" t="n">
-        <v>-214</v>
+        <v>45</v>
       </c>
       <c r="F48" t="n">
-        <v>45</v>
-      </c>
-      <c r="G48" t="n">
         <v>33</v>
       </c>
-      <c r="H48" t="inlineStr"/>
-      <c r="I48" t="n">
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="n">
         <v>-208</v>
       </c>
     </row>
@@ -3746,23 +3508,20 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>39</v>
-      </c>
-      <c r="C49" t="n">
         <v>45</v>
       </c>
-      <c r="D49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="n">
+        <v>-222</v>
+      </c>
       <c r="E49" t="n">
-        <v>-222</v>
+        <v>-206</v>
       </c>
       <c r="F49" t="n">
-        <v>-206</v>
-      </c>
-      <c r="G49" t="n">
         <v>36</v>
       </c>
-      <c r="H49" t="inlineStr"/>
-      <c r="I49" t="n">
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="n">
         <v>44</v>
       </c>
     </row>
@@ -3771,23 +3530,20 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>48</v>
-      </c>
-      <c r="C50" t="n">
         <v>46</v>
       </c>
-      <c r="D50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="n">
+        <v>-238</v>
+      </c>
       <c r="E50" t="n">
-        <v>-238</v>
+        <v>-208</v>
       </c>
       <c r="F50" t="n">
-        <v>-208</v>
-      </c>
-      <c r="G50" t="n">
         <v>37</v>
       </c>
-      <c r="H50" t="inlineStr"/>
-      <c r="I50" t="n">
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="n">
         <v>44</v>
       </c>
     </row>
@@ -3798,21 +3554,18 @@
       <c r="B51" t="n">
         <v>48</v>
       </c>
-      <c r="C51" t="n">
-        <v>48</v>
-      </c>
-      <c r="D51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="n">
+        <v>-218</v>
+      </c>
       <c r="E51" t="n">
-        <v>-218</v>
+        <v>-208</v>
       </c>
       <c r="F51" t="n">
-        <v>-208</v>
-      </c>
-      <c r="G51" t="n">
         <v>32</v>
       </c>
-      <c r="H51" t="inlineStr"/>
-      <c r="I51" t="n">
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="n">
         <v>-206</v>
       </c>
     </row>
@@ -3821,23 +3574,20 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>47</v>
-      </c>
-      <c r="C52" t="n">
         <v>48</v>
       </c>
-      <c r="D52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="n">
+        <v>-214</v>
+      </c>
       <c r="E52" t="n">
-        <v>-214</v>
+        <v>45</v>
       </c>
       <c r="F52" t="n">
-        <v>45</v>
-      </c>
-      <c r="G52" t="n">
         <v>35</v>
       </c>
-      <c r="H52" t="inlineStr"/>
-      <c r="I52" t="n">
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="n">
         <v>46</v>
       </c>
     </row>
@@ -3846,23 +3596,20 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>48</v>
-      </c>
-      <c r="C53" t="n">
         <v>-206</v>
       </c>
-      <c r="D53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="n">
+        <v>-214</v>
+      </c>
       <c r="E53" t="n">
-        <v>-214</v>
+        <v>-210</v>
       </c>
       <c r="F53" t="n">
-        <v>-210</v>
-      </c>
-      <c r="G53" t="n">
         <v>37</v>
       </c>
+      <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
-      <c r="I53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -3871,90 +3618,78 @@
       <c r="B54" t="n">
         <v>47</v>
       </c>
-      <c r="C54" t="n">
-        <v>47</v>
-      </c>
-      <c r="D54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="n">
+        <v>-214</v>
+      </c>
       <c r="E54" t="n">
-        <v>-214</v>
+        <v>-218</v>
       </c>
       <c r="F54" t="n">
-        <v>-218</v>
-      </c>
-      <c r="G54" t="n">
         <v>4</v>
       </c>
+      <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr"/>
-      <c r="I54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>25</v>
-      </c>
-      <c r="C55" t="n">
         <v>48</v>
       </c>
-      <c r="D55" t="inlineStr"/>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="n">
+        <v>-214</v>
+      </c>
       <c r="E55" t="n">
-        <v>-214</v>
+        <v>46</v>
       </c>
       <c r="F55" t="n">
-        <v>46</v>
-      </c>
-      <c r="G55" t="n">
         <v>43</v>
       </c>
+      <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
-      <c r="I55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>45</v>
-      </c>
-      <c r="C56" t="n">
-        <v>47</v>
-      </c>
-      <c r="D56" t="inlineStr"/>
+        <v>47</v>
+      </c>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="n">
+        <v>-214</v>
+      </c>
       <c r="E56" t="n">
-        <v>-214</v>
+        <v>-208</v>
       </c>
       <c r="F56" t="n">
-        <v>-208</v>
-      </c>
-      <c r="G56" t="n">
         <v>-248</v>
       </c>
+      <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr"/>
-      <c r="I56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>-220</v>
-      </c>
-      <c r="C57" t="n">
-        <v>47</v>
-      </c>
-      <c r="D57" t="inlineStr"/>
+        <v>47</v>
+      </c>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="n">
+        <v>-214</v>
+      </c>
       <c r="E57" t="n">
-        <v>-214</v>
+        <v>-208</v>
       </c>
       <c r="F57" t="n">
-        <v>-208</v>
-      </c>
-      <c r="G57" t="n">
         <v>-226</v>
       </c>
+      <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
-      <c r="I57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -3963,145 +3698,138 @@
       <c r="B58" t="n">
         <v>48</v>
       </c>
-      <c r="C58" t="n">
-        <v>48</v>
-      </c>
-      <c r="D58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="n">
+        <v>-214</v>
+      </c>
       <c r="E58" t="n">
-        <v>-214</v>
+        <v>45</v>
       </c>
       <c r="F58" t="n">
-        <v>45</v>
-      </c>
-      <c r="G58" t="n">
         <v>-226</v>
       </c>
+      <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>47</v>
-      </c>
-      <c r="C59" t="n">
         <v>48</v>
       </c>
-      <c r="D59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="n">
+        <v>-220</v>
+      </c>
       <c r="E59" t="n">
-        <v>-220</v>
+        <v>46</v>
       </c>
       <c r="F59" t="n">
-        <v>46</v>
-      </c>
-      <c r="G59" t="n">
-        <v>47</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
-      <c r="I59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
       <c r="B60" t="n">
+        <v>48</v>
+      </c>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="n">
+        <v>33</v>
+      </c>
+      <c r="E60" t="n">
         <v>45</v>
       </c>
-      <c r="C60" t="n">
-        <v>48</v>
-      </c>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="n">
-        <v>33</v>
-      </c>
       <c r="F60" t="n">
-        <v>45</v>
-      </c>
-      <c r="G60" t="n">
         <v>43</v>
       </c>
+      <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr"/>
-      <c r="I60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>41</v>
+        <v>-214</v>
       </c>
       <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
+      <c r="D61" t="n">
+        <v>-214</v>
+      </c>
       <c r="E61" t="n">
-        <v>-214</v>
+        <v>-210</v>
       </c>
       <c r="F61" t="n">
-        <v>-210</v>
-      </c>
-      <c r="G61" t="n">
         <v>30</v>
       </c>
+      <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
-      <c r="I61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="B62" t="inlineStr"/>
+      <c r="B62" t="n">
+        <v>-212</v>
+      </c>
       <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
+      <c r="D62" t="n">
+        <v>-220</v>
+      </c>
       <c r="E62" t="n">
-        <v>-220</v>
+        <v>-206</v>
       </c>
       <c r="F62" t="n">
-        <v>-206</v>
-      </c>
-      <c r="G62" t="n">
         <v>43</v>
       </c>
+      <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
-      <c r="I62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="B63" t="inlineStr"/>
+      <c r="B63" t="n">
+        <v>-208</v>
+      </c>
       <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
+      <c r="D63" t="n">
+        <v>46</v>
+      </c>
       <c r="E63" t="n">
-        <v>46</v>
+        <v>-218</v>
       </c>
       <c r="F63" t="n">
-        <v>-218</v>
-      </c>
-      <c r="G63" t="n">
         <v>45</v>
       </c>
+      <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
-      <c r="I63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="B64" t="inlineStr"/>
+      <c r="B64" t="n">
+        <v>47</v>
+      </c>
       <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
+      <c r="D64" t="n">
+        <v>-214</v>
+      </c>
       <c r="E64" t="n">
-        <v>-214</v>
+        <v>45</v>
       </c>
       <c r="F64" t="n">
-        <v>45</v>
-      </c>
-      <c r="G64" t="n">
         <v>33</v>
       </c>
+      <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
-      <c r="I64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -4109,18 +3837,17 @@
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr"/>
+      <c r="D65" t="n">
+        <v>-214</v>
+      </c>
       <c r="E65" t="n">
+        <v>45</v>
+      </c>
+      <c r="F65" t="n">
         <v>-214</v>
       </c>
-      <c r="F65" t="n">
-        <v>45</v>
-      </c>
-      <c r="G65" t="n">
-        <v>-214</v>
-      </c>
+      <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
-      <c r="I65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
@@ -4128,18 +3855,17 @@
       </c>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr"/>
+      <c r="D66" t="n">
+        <v>-214</v>
+      </c>
       <c r="E66" t="n">
-        <v>-214</v>
+        <v>-210</v>
       </c>
       <c r="F66" t="n">
-        <v>-210</v>
-      </c>
-      <c r="G66" t="n">
         <v>43</v>
       </c>
+      <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
-      <c r="I66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -4147,18 +3873,17 @@
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr"/>
+      <c r="D67" t="n">
+        <v>12</v>
+      </c>
       <c r="E67" t="n">
-        <v>12</v>
+        <v>-210</v>
       </c>
       <c r="F67" t="n">
-        <v>-210</v>
-      </c>
-      <c r="G67" t="n">
         <v>-274</v>
       </c>
+      <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
-      <c r="I67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -4166,16 +3891,17 @@
       </c>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr"/>
+      <c r="D68" t="n">
+        <v>-224</v>
+      </c>
+      <c r="E68" t="n">
+        <v>43</v>
+      </c>
       <c r="F68" t="n">
-        <v>43</v>
-      </c>
-      <c r="G68" t="n">
         <v>37</v>
       </c>
+      <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
-      <c r="I68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
@@ -4183,16 +3909,17 @@
       </c>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr"/>
+      <c r="D69" t="n">
+        <v>-208</v>
+      </c>
+      <c r="E69" t="n">
+        <v>43</v>
+      </c>
       <c r="F69" t="n">
-        <v>43</v>
-      </c>
-      <c r="G69" t="n">
         <v>-272</v>
       </c>
+      <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
-      <c r="I69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -4200,16 +3927,17 @@
       </c>
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr"/>
+      <c r="D70" t="n">
+        <v>-27</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-208</v>
+      </c>
       <c r="F70" t="n">
-        <v>-208</v>
-      </c>
-      <c r="G70" t="n">
         <v>37</v>
       </c>
+      <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr"/>
-      <c r="I70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
@@ -4217,16 +3945,17 @@
       </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr"/>
+      <c r="D71" t="n">
+        <v>46</v>
+      </c>
+      <c r="E71" t="n">
+        <v>45</v>
+      </c>
       <c r="F71" t="n">
-        <v>45</v>
-      </c>
-      <c r="G71" t="n">
         <v>26</v>
       </c>
+      <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
-      <c r="I71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -4235,15 +3964,14 @@
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr"/>
       <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr"/>
+      <c r="E72" t="n">
+        <v>-214</v>
+      </c>
       <c r="F72" t="n">
-        <v>-214</v>
-      </c>
-      <c r="G72" t="n">
         <v>-212</v>
       </c>
+      <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
-      <c r="I72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -4252,15 +3980,14 @@
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr"/>
       <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr"/>
+      <c r="E73" t="n">
+        <v>46</v>
+      </c>
       <c r="F73" t="n">
-        <v>46</v>
-      </c>
-      <c r="G73" t="n">
         <v>21</v>
       </c>
+      <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
-      <c r="I73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -4269,15 +3996,14 @@
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr"/>
       <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr"/>
+      <c r="E74" t="n">
+        <v>-210</v>
+      </c>
       <c r="F74" t="n">
-        <v>-210</v>
-      </c>
-      <c r="G74" t="n">
         <v>42</v>
       </c>
+      <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
-      <c r="I74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -4286,15 +4012,14 @@
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr"/>
       <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
+      <c r="E75" t="n">
+        <v>46</v>
+      </c>
       <c r="F75" t="n">
-        <v>46</v>
-      </c>
-      <c r="G75" t="n">
         <v>-222</v>
       </c>
+      <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
-      <c r="I75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
@@ -4303,15 +4028,14 @@
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr"/>
       <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr"/>
+      <c r="E76" t="n">
+        <v>-208</v>
+      </c>
       <c r="F76" t="n">
-        <v>-208</v>
-      </c>
-      <c r="G76" t="n">
         <v>41</v>
       </c>
+      <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
-      <c r="I76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -4320,15 +4044,14 @@
       <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr"/>
       <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr"/>
+      <c r="E77" t="n">
+        <v>-214</v>
+      </c>
       <c r="F77" t="n">
-        <v>-214</v>
-      </c>
-      <c r="G77" t="n">
         <v>37</v>
       </c>
+      <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
-      <c r="I77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -4337,15 +4060,72 @@
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr"/>
       <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
+      <c r="E78" t="n">
+        <v>-208</v>
+      </c>
       <c r="F78" t="n">
-        <v>-208</v>
-      </c>
-      <c r="G78" t="n">
         <v>36</v>
       </c>
+      <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
-      <c r="I78" t="inlineStr"/>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="n">
+        <v>-210</v>
+      </c>
+      <c r="F79" t="n">
+        <v>-220</v>
+      </c>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="n">
+        <v>-204</v>
+      </c>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
+      <c r="E81" t="n">
+        <v>-214</v>
+      </c>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr"/>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="n">
+        <v>-210</v>
+      </c>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>